<commit_message>
BOM finished except for res and cap part numbers. Need to check DNPs, 0 ohms, and crystals.
</commit_message>
<xml_diff>
--- a/CANnode/Output/BOM_Final.xlsx
+++ b/CANnode/Output/BOM_Final.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="199">
   <si>
     <t>Qty</t>
   </si>
@@ -36,9 +36,6 @@
     <t>Device</t>
   </si>
   <si>
-    <t>CHIP-LED</t>
-  </si>
-  <si>
     <t>DSOD323</t>
   </si>
   <si>
@@ -81,9 +78,6 @@
     <t>1k</t>
   </si>
   <si>
-    <t>R-US_R0402</t>
-  </si>
-  <si>
     <t>R40, R66, R67, R68, R69, R77, R78, R79</t>
   </si>
   <si>
@@ -252,12 +246,6 @@
     <t>X1</t>
   </si>
   <si>
-    <t>Blue</t>
-  </si>
-  <si>
-    <t>D26</t>
-  </si>
-  <si>
     <t>DNP</t>
   </si>
   <si>
@@ -313,12 +301,6 @@
   </si>
   <si>
     <t>U$5</t>
-  </si>
-  <si>
-    <t>VARISTORCN0805</t>
-  </si>
-  <si>
-    <t>R4</t>
   </si>
   <si>
     <t>XC2C32A-6CP56C</t>
@@ -423,9 +405,6 @@
     <t>D28</t>
   </si>
   <si>
-    <t>D27</t>
-  </si>
-  <si>
     <t>CHIP-LED-YELLOW</t>
   </si>
   <si>
@@ -556,6 +535,96 @@
   </si>
   <si>
     <t>20V</t>
+  </si>
+  <si>
+    <t>Microchip Technology</t>
+  </si>
+  <si>
+    <t>IC EEPROM 2KBIT 3MHZ 8SOIC</t>
+  </si>
+  <si>
+    <t>8-SOIC</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Fairchild Semiconductor</t>
+  </si>
+  <si>
+    <t>MOSFET P-CH 25V 120MA SOT-23</t>
+  </si>
+  <si>
+    <t>SOT-23</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> FTDI, Future Technology Devices International Ltd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IC USB HS DUAL UART/FIFO 64-LQFP </t>
+  </si>
+  <si>
+    <t>64-LQFP</t>
+  </si>
+  <si>
+    <t>IC TXRX CAN 5V 8SOP</t>
+  </si>
+  <si>
+    <t>8-SOP</t>
+  </si>
+  <si>
+    <t>ISO1050DUBR</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Texas Instruments</t>
+  </si>
+  <si>
+    <t>IC OPAMP GP 1.2MHZ 14TSSOP</t>
+  </si>
+  <si>
+    <t>14-TSSOP</t>
+  </si>
+  <si>
+    <t>RM42L432BPZT</t>
+  </si>
+  <si>
+    <t>IC MCU 16BIT 384KB FLASH 100LQFP</t>
+  </si>
+  <si>
+    <t>100-LQFP</t>
+  </si>
+  <si>
+    <t>TPS70445PWP</t>
+  </si>
+  <si>
+    <t>IC REG LDO 3.3V/1.2V 24HTSSOP</t>
+  </si>
+  <si>
+    <t>24-HTSSOP</t>
+  </si>
+  <si>
+    <t>D26, D27</t>
+  </si>
+  <si>
+    <t>Autosport connector</t>
+  </si>
+  <si>
+    <t>AS214-35-PN</t>
+  </si>
+  <si>
+    <t>Deutch</t>
+  </si>
+  <si>
+    <t>do not populate</t>
+  </si>
+  <si>
+    <t>Xilinx Inc.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> IC CPLD 32MC 5.5NS 56BGA</t>
+  </si>
+  <si>
+    <t>56-LFBGA, CSPBGA</t>
+  </si>
+  <si>
+    <t>possibe replacment:  XC2C64A-7CPG56I</t>
   </si>
 </sst>
 </file>
@@ -670,7 +739,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -707,6 +776,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -773,8 +843,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:K57" totalsRowShown="0">
-  <autoFilter ref="A1:K57"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:K55" totalsRowShown="0">
+  <autoFilter ref="A1:K55"/>
   <sortState ref="A2:K56">
     <sortCondition ref="J2:J55" customList=".01uF,.1uF,.1uF,0R,0ZCJ0050AF2E,100K,100k,100nF,100nF,100nF,10K,120R,12K,12M,1751316,1K,1k,1uF,1uF,2.2K,20.1K,20.1k,200,200R,22,220R @ 100M,22pF,22uF,250,250k,39K,4.7K,4.7uF,47uF,698,7M-16.000MAAJ-T,93LC56C-I/SN"/>
   </sortState>
@@ -1058,10 +1128,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K57"/>
+  <dimension ref="A1:L55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="K54" sqref="K54"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L48" sqref="L48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1077,36 +1147,37 @@
     <col min="9" max="9" width="18.140625" style="7" customWidth="1"/>
     <col min="10" max="10" width="25.42578125" style="6" customWidth="1"/>
     <col min="11" max="11" width="19.85546875" style="6" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="6"/>
+    <col min="12" max="12" width="40.140625" style="6" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="G1" s="11" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="J1" s="2" t="s">
         <v>1</v>
@@ -1117,7 +1188,7 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B2" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C2" s="8">
         <v>8</v>
@@ -1127,21 +1198,21 @@
         <v>CAP .01uF 0402</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B3" s="8" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="C3" s="8">
         <v>4</v>
@@ -1151,21 +1222,21 @@
         <v>CAP .1uF 0402</v>
       </c>
       <c r="G3" s="12" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B4" s="8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C4" s="8">
         <v>11</v>
@@ -1175,50 +1246,50 @@
         <v>RES 0R 0402</v>
       </c>
       <c r="G4" s="12" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="J4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K4" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B5" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C5" s="8">
         <v>1</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="E5" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="G5" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K5" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="F5" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="G5" s="12" t="s">
-        <v>116</v>
-      </c>
-      <c r="H5" s="7" t="s">
-        <v>120</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="K5" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B6" s="8" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C6" s="8">
         <v>1</v>
@@ -1228,21 +1299,21 @@
         <v>RES 100K 0402</v>
       </c>
       <c r="G6" s="12" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B7" s="8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C7" s="8">
         <v>1</v>
@@ -1252,21 +1323,21 @@
         <v>RES 100k 0402</v>
       </c>
       <c r="G7" s="12" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B8" s="8" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C8" s="8">
         <v>14</v>
@@ -1276,21 +1347,21 @@
         <v>CAP 100nF 0402</v>
       </c>
       <c r="G8" s="12" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B9" s="8" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C9" s="8">
         <v>16</v>
@@ -1300,21 +1371,21 @@
         <v>CAP 100nF 0402</v>
       </c>
       <c r="G9" s="12" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="H9" s="7" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B10" s="8" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C10" s="8">
         <v>2</v>
@@ -1324,21 +1395,21 @@
         <v>CAP 100nF 0402</v>
       </c>
       <c r="G10" s="12" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="H10" s="7" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B11" s="8" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C11" s="8">
         <v>2</v>
@@ -1348,21 +1419,21 @@
         <v>RES 10K 0402</v>
       </c>
       <c r="G11" s="12" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B12" s="8" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C12" s="8">
         <v>1</v>
@@ -1372,103 +1443,103 @@
         <v>RES 120R 0402</v>
       </c>
       <c r="G12" s="12" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="H12" s="7" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B13" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" s="8">
+        <v>1</v>
+      </c>
+      <c r="F13" s="7" t="str">
+        <f>CONCATENATE(LEFT(Table1[[#This Row],[Device]],3)," ",Table1[[#This Row],[Value]]," ",RIGHT(Table1[[#This Row],[Device]],4))</f>
+        <v>RES 12K 0402</v>
+      </c>
+      <c r="G13" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="H13" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="15"/>
+      <c r="B14" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" s="16">
+        <v>1</v>
+      </c>
+      <c r="D14" s="15" t="s">
+        <v>116</v>
+      </c>
+      <c r="E14" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="F14" s="15" t="s">
+        <v>117</v>
+      </c>
+      <c r="G14" s="17" t="s">
+        <v>118</v>
+      </c>
+      <c r="H14" s="15"/>
+      <c r="I14" s="15"/>
+      <c r="J14" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="K14" s="18" t="s">
         <v>34</v>
-      </c>
-      <c r="C13" s="8">
-        <v>1</v>
-      </c>
-      <c r="F13" s="7" t="str">
-        <f>CONCATENATE(LEFT(Table1[[#This Row],[Device]],3)," ",Table1[[#This Row],[Value]]," ",RIGHT(Table1[[#This Row],[Device]],4))</f>
-        <v>RES 12K 0402</v>
-      </c>
-      <c r="G13" s="12" t="s">
-        <v>115</v>
-      </c>
-      <c r="H13" s="7" t="s">
-        <v>120</v>
-      </c>
-      <c r="J13" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="K13" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="14"/>
-      <c r="B14" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="C14" s="15">
-        <v>1</v>
-      </c>
-      <c r="D14" s="14" t="s">
-        <v>122</v>
-      </c>
-      <c r="E14" s="14" t="s">
-        <v>121</v>
-      </c>
-      <c r="F14" s="14" t="s">
-        <v>123</v>
-      </c>
-      <c r="G14" s="16" t="s">
-        <v>124</v>
-      </c>
-      <c r="H14" s="14"/>
-      <c r="I14" s="14"/>
-      <c r="J14" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="K14" s="17" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B15" s="8" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C15" s="8">
         <v>1</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="E15" s="13">
         <v>1751316</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="G15" s="12" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="H15" s="7" t="s">
-        <v>127</v>
-      </c>
-      <c r="J15" s="18">
+        <v>121</v>
+      </c>
+      <c r="J15" s="19">
         <v>1751316</v>
       </c>
-      <c r="K15" s="18">
+      <c r="K15" s="19">
         <v>1751316</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B16" s="8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C16" s="8">
         <v>4</v>
@@ -1478,21 +1549,21 @@
         <v>RES 1K 0402</v>
       </c>
       <c r="G16" s="12" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="H16" s="7" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B17" s="8" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C17" s="8">
         <v>8</v>
@@ -1502,21 +1573,21 @@
         <v>RES 1k 0402</v>
       </c>
       <c r="G17" s="12" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="H17" s="7" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="18" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B18" s="8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C18" s="8">
         <v>16</v>
@@ -1526,21 +1597,21 @@
         <v>CAP 1uF 0402</v>
       </c>
       <c r="G18" s="12" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="H18" s="7" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="19" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B19" s="8" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C19" s="8">
         <v>2</v>
@@ -1550,21 +1621,21 @@
         <v>CAP 1uF 0402</v>
       </c>
       <c r="G19" s="12" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="H19" s="7" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="20" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B20" s="8" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C20" s="8">
         <v>1</v>
@@ -1574,21 +1645,21 @@
         <v>RES 2.2K 0402</v>
       </c>
       <c r="G20" s="12" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="H20" s="7" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="21" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B21" s="8" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C21" s="8">
         <v>1</v>
@@ -1598,21 +1669,21 @@
         <v>RES 20.1K 0402</v>
       </c>
       <c r="G21" s="12" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="H21" s="7" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="K21" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="22" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B22" s="8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C22" s="8">
         <v>23</v>
@@ -1622,21 +1693,21 @@
         <v>RES 20.1k 0402</v>
       </c>
       <c r="G22" s="12" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="H22" s="7" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="23" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B23" s="8" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C23" s="8">
         <v>1</v>
@@ -1646,21 +1717,21 @@
         <v>RES 200 0402</v>
       </c>
       <c r="G23" s="12" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="H23" s="7" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="J23" s="1">
         <v>200</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="24" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B24" s="8" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C24" s="8">
         <v>2</v>
@@ -1670,21 +1741,21 @@
         <v>RES 200R 0402</v>
       </c>
       <c r="G24" s="12" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="H24" s="7" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="K24" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="25" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B25" s="8" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C25" s="8">
         <v>2</v>
@@ -1694,50 +1765,50 @@
         <v>RES 22 0402</v>
       </c>
       <c r="G25" s="12" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="H25" s="7" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="J25" s="1">
         <v>22</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="26" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B26" s="8" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C26" s="8">
         <v>2</v>
       </c>
       <c r="D26" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="E26" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="F26" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="G26" s="12" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="H26" s="7" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="27" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B27" s="8" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="C27" s="8">
         <v>4</v>
@@ -1747,21 +1818,21 @@
         <v>CAP 22pF 0402</v>
       </c>
       <c r="G27" s="12" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="H27" s="7" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="J27" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="K27" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="28" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B28" s="8" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="C28" s="8">
         <v>2</v>
@@ -1771,50 +1842,50 @@
         <v>CAP 22uF 0402</v>
       </c>
       <c r="G28" s="12" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="H28" s="7" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="J28" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="K28" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="29" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B29" s="8" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C29" s="8">
         <v>1</v>
       </c>
       <c r="D29" s="7" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="E29" s="7" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="F29" s="7" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="G29" s="12" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="H29" s="7" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="J29" s="1">
         <v>619</v>
       </c>
       <c r="K29" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="30" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B30" s="8" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C30" s="8">
         <v>2</v>
@@ -1824,21 +1895,21 @@
         <v>RES 250k 0402</v>
       </c>
       <c r="G30" s="12" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="H30" s="7" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="J30" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="K30" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="31" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B31" s="8" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C31" s="8">
         <v>25</v>
@@ -1848,21 +1919,21 @@
         <v>RES 39K 0402</v>
       </c>
       <c r="G31" s="12" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="H31" s="7" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="J31" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="K31" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="32" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B32" s="8" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C32" s="8">
         <v>4</v>
@@ -1872,21 +1943,21 @@
         <v>RES 4.7K 0402</v>
       </c>
       <c r="G32" s="12" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="H32" s="7" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="J32" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="K32" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B33" s="8" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="C33" s="8">
         <v>7</v>
@@ -1896,21 +1967,21 @@
         <v>CAP 4.7uF 0805</v>
       </c>
       <c r="G33" s="12" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="H33" s="7" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="J33" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="K33" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B34" s="8" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C34" s="8">
         <v>1</v>
@@ -1920,21 +1991,21 @@
         <v>CAP 47uF 0402</v>
       </c>
       <c r="G34" s="12" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="H34" s="7" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="J34" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="K34" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B35" s="8" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C35" s="8">
         <v>16</v>
@@ -1944,471 +2015,575 @@
         <v>RES 698 0402</v>
       </c>
       <c r="G35" s="12" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="H35" s="7" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="J35" s="1">
         <v>698</v>
       </c>
       <c r="K35" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A36" s="14"/>
-      <c r="B36" s="15" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A36" s="15"/>
+      <c r="B36" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="C36" s="16">
+        <v>1</v>
+      </c>
+      <c r="D36" s="15" t="s">
+        <v>116</v>
+      </c>
+      <c r="E36" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="F36" s="15" t="s">
+        <v>117</v>
+      </c>
+      <c r="G36" s="17" t="s">
+        <v>118</v>
+      </c>
+      <c r="H36" s="15"/>
+      <c r="I36" s="15"/>
+      <c r="J36" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="K36" s="18" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B37" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="C37" s="8">
+        <v>1</v>
+      </c>
+      <c r="D37" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="E37" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="F37" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="G37" s="12" t="s">
+        <v>171</v>
+      </c>
+      <c r="H37" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="J37" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="K37" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B38" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="C38" s="8">
+        <v>1</v>
+      </c>
+      <c r="D38" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="E38" s="7" t="s">
+        <v>192</v>
+      </c>
+      <c r="F38" s="7" t="s">
+        <v>191</v>
+      </c>
+      <c r="I38" s="7" t="s">
+        <v>194</v>
+      </c>
+      <c r="J38" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="K38" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B39" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="C39" s="8">
+        <v>3</v>
+      </c>
+      <c r="J39" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="K39" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B40" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="C40" s="8">
+        <v>2</v>
+      </c>
+      <c r="D40" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="E40" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="F40" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="G40" s="12" t="s">
+        <v>174</v>
+      </c>
+      <c r="H40" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="J40" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="K40" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B41" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="C41" s="8">
+        <v>1</v>
+      </c>
+      <c r="D41" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="F41" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="G41" s="12" t="s">
+        <v>177</v>
+      </c>
+      <c r="H41" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="J41" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="K41" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B42" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="C42" s="8">
+        <v>2</v>
+      </c>
+      <c r="D42" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="E42" s="7" t="s">
+        <v>180</v>
+      </c>
+      <c r="F42" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="G42" s="12" t="s">
+        <v>179</v>
+      </c>
+      <c r="H42" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="J42" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="K42" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B43" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="C43" s="8">
+        <v>6</v>
+      </c>
+      <c r="D43" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="F43" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="G43" s="12" t="s">
+        <v>183</v>
+      </c>
+      <c r="H43" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="J43" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="K43" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="B44" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="C44" s="8">
+        <v>1</v>
+      </c>
+      <c r="D44" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="E44" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="F44" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="G44" s="12" t="s">
+        <v>186</v>
+      </c>
+      <c r="H44" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="J44" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="K44" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B45" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="C45" s="8">
+        <v>1</v>
+      </c>
+      <c r="D45" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="E45" s="7" t="s">
+        <v>187</v>
+      </c>
+      <c r="F45" s="14" t="s">
+        <v>188</v>
+      </c>
+      <c r="G45" s="12" t="s">
+        <v>189</v>
+      </c>
+      <c r="H45" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="J45" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="K45" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B46" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="C46" s="8">
         <v>30</v>
       </c>
-      <c r="C36" s="15">
-        <v>1</v>
-      </c>
-      <c r="D36" s="14" t="s">
-        <v>122</v>
-      </c>
-      <c r="E36" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="F36" s="14" t="s">
-        <v>123</v>
-      </c>
-      <c r="G36" s="16" t="s">
-        <v>124</v>
-      </c>
-      <c r="H36" s="14"/>
-      <c r="I36" s="14"/>
-      <c r="J36" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="K36" s="17" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B37" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="C37" s="8">
-        <v>1</v>
-      </c>
-      <c r="J37" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="K37" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B38" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="C38" s="8">
-        <v>1</v>
-      </c>
-      <c r="J38" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="K38" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B39" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="C39" s="8">
-        <v>1</v>
-      </c>
-      <c r="H39" s="7" t="s">
-        <v>120</v>
-      </c>
-      <c r="J39" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="K39" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B40" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="C40" s="8">
-        <v>3</v>
-      </c>
-      <c r="J40" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="K40" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B41" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="C41" s="8">
-        <v>2</v>
-      </c>
-      <c r="J41" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="K41" s="1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B42" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="C42" s="8">
-        <v>1</v>
-      </c>
-      <c r="J42" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="K42" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B43" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="C43" s="8">
-        <v>2</v>
-      </c>
-      <c r="J43" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="K43" s="1" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B44" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="C44" s="8">
-        <v>6</v>
-      </c>
-      <c r="J44" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="K44" s="1" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="45" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="B45" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="C45" s="8">
-        <v>1</v>
-      </c>
-      <c r="J45" s="1" t="s">
+      <c r="D46" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="E46" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="F46" s="20" t="s">
+        <v>144</v>
+      </c>
+      <c r="G46" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="H46" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="J46" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="K45" s="1" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B46" s="8" t="s">
+      <c r="K46" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="B47" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="C46" s="8">
-        <v>1</v>
-      </c>
-      <c r="J46" s="1" t="s">
+      <c r="C47" s="8">
+        <v>1</v>
+      </c>
+      <c r="D47" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="E47" s="7">
+        <v>1050170001</v>
+      </c>
+      <c r="F47" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="G47" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="H47" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="J47" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="K46" s="1" t="s">
+      <c r="K47" s="1" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B47" s="8" t="s">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B48" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="C47" s="8">
-        <v>30</v>
-      </c>
-      <c r="D47" s="7" t="s">
-        <v>150</v>
-      </c>
-      <c r="E47" s="7" t="s">
-        <v>149</v>
-      </c>
-      <c r="F47" s="19" t="s">
-        <v>151</v>
-      </c>
-      <c r="G47" s="12" t="s">
-        <v>115</v>
-      </c>
-      <c r="H47" s="7" t="s">
-        <v>120</v>
-      </c>
-      <c r="J47" s="1" t="s">
+      <c r="C48" s="8">
+        <v>1</v>
+      </c>
+      <c r="D48" s="7" t="s">
+        <v>195</v>
+      </c>
+      <c r="E48" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="K47" s="1" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="48" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="B48" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="C48" s="8">
-        <v>1</v>
-      </c>
-      <c r="D48" s="7" t="s">
-        <v>146</v>
-      </c>
-      <c r="E48" s="7">
-        <v>1050170001</v>
-      </c>
       <c r="F48" s="7" t="s">
-        <v>147</v>
+        <v>196</v>
       </c>
       <c r="G48" s="12" t="s">
-        <v>148</v>
+        <v>197</v>
       </c>
       <c r="H48" s="7" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="J48" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="K48" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
+      </c>
+      <c r="L48" s="6" t="s">
+        <v>198</v>
       </c>
     </row>
     <row r="49" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B49" s="8" t="s">
-        <v>97</v>
+        <v>190</v>
       </c>
       <c r="C49" s="8">
         <v>1</v>
       </c>
+      <c r="D49" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="E49" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="F49" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="G49" s="12" t="s">
+        <v>108</v>
+      </c>
+      <c r="H49" s="7" t="s">
+        <v>114</v>
+      </c>
       <c r="J49" s="1" t="s">
-        <v>96</v>
+        <v>130</v>
       </c>
       <c r="K49" s="1" t="s">
-        <v>96</v>
+        <v>126</v>
       </c>
     </row>
     <row r="50" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B50" s="8" t="s">
-        <v>99</v>
+        <v>124</v>
       </c>
       <c r="C50" s="8">
         <v>1</v>
       </c>
+      <c r="D50" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="E50" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="F50" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="G50" s="12" t="s">
+        <v>108</v>
+      </c>
+      <c r="H50" s="7" t="s">
+        <v>114</v>
+      </c>
       <c r="J50" s="1" t="s">
-        <v>98</v>
+        <v>131</v>
       </c>
       <c r="K50" s="1" t="s">
-        <v>98</v>
+        <v>125</v>
       </c>
     </row>
     <row r="51" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B51" s="8" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="C51" s="8">
         <v>1</v>
       </c>
       <c r="D51" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="E51" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="F51" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="G51" s="12" t="s">
+        <v>108</v>
+      </c>
+      <c r="H51" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="J51" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="K51" s="10" t="s">
         <v>135</v>
-      </c>
-      <c r="E51" s="7" t="s">
-        <v>140</v>
-      </c>
-      <c r="F51" s="7" t="s">
-        <v>139</v>
-      </c>
-      <c r="G51" s="12" t="s">
-        <v>114</v>
-      </c>
-      <c r="H51" s="7" t="s">
-        <v>120</v>
-      </c>
-      <c r="J51" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="K51" s="1" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="52" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B52" s="8" t="s">
-        <v>130</v>
+        <v>4</v>
       </c>
       <c r="C52" s="8">
         <v>1</v>
       </c>
       <c r="D52" s="7" t="s">
-        <v>135</v>
+        <v>166</v>
       </c>
       <c r="E52" s="7" t="s">
-        <v>134</v>
+        <v>164</v>
       </c>
       <c r="F52" s="7" t="s">
-        <v>136</v>
+        <v>165</v>
       </c>
       <c r="G52" s="12" t="s">
-        <v>114</v>
+        <v>167</v>
       </c>
       <c r="H52" s="7" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="J52" s="1" t="s">
-        <v>138</v>
+        <v>168</v>
       </c>
       <c r="K52" s="1" t="s">
-        <v>132</v>
+        <v>3</v>
       </c>
     </row>
     <row r="53" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B53" s="8" t="s">
-        <v>129</v>
+        <v>158</v>
       </c>
       <c r="C53" s="8">
         <v>1</v>
       </c>
       <c r="D53" s="7" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="E53" s="7" t="s">
-        <v>143</v>
+        <v>159</v>
       </c>
       <c r="F53" s="7" t="s">
-        <v>145</v>
+        <v>160</v>
       </c>
       <c r="G53" s="12" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="H53" s="7" t="s">
-        <v>120</v>
-      </c>
-      <c r="J53" s="9" t="s">
-        <v>141</v>
+        <v>114</v>
+      </c>
+      <c r="J53" s="1" t="s">
+        <v>134</v>
       </c>
       <c r="K53" s="10" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
     </row>
     <row r="54" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B54" s="8" t="s">
-        <v>5</v>
+        <v>146</v>
       </c>
       <c r="C54" s="8">
         <v>1</v>
       </c>
       <c r="D54" s="7" t="s">
-        <v>173</v>
+        <v>148</v>
       </c>
       <c r="E54" s="7" t="s">
-        <v>171</v>
+        <v>149</v>
       </c>
       <c r="F54" s="7" t="s">
-        <v>172</v>
-      </c>
-      <c r="G54" s="12" t="s">
-        <v>174</v>
+        <v>147</v>
       </c>
       <c r="H54" s="7" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="J54" s="1" t="s">
-        <v>175</v>
+        <v>151</v>
       </c>
       <c r="K54" s="1" t="s">
-        <v>4</v>
+        <v>150</v>
       </c>
     </row>
     <row r="55" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B55" s="8" t="s">
-        <v>165</v>
+        <v>152</v>
       </c>
       <c r="C55" s="8">
         <v>1</v>
       </c>
       <c r="D55" s="7" t="s">
-        <v>144</v>
+        <v>154</v>
       </c>
       <c r="E55" s="7" t="s">
-        <v>166</v>
+        <v>153</v>
       </c>
       <c r="F55" s="7" t="s">
-        <v>167</v>
-      </c>
-      <c r="G55" s="12" t="s">
-        <v>115</v>
+        <v>155</v>
       </c>
       <c r="H55" s="7" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="J55" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="K55" s="10" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="56" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B56" s="8" t="s">
-        <v>153</v>
-      </c>
-      <c r="C56" s="8">
-        <v>1</v>
-      </c>
-      <c r="D56" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="E56" s="7" t="s">
         <v>156</v>
       </c>
-      <c r="F56" s="7" t="s">
-        <v>154</v>
-      </c>
-      <c r="H56" s="7" t="s">
-        <v>120</v>
-      </c>
-      <c r="J56" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="K56" s="1" t="s">
+      <c r="K55" s="1" t="s">
         <v>157</v>
-      </c>
-    </row>
-    <row r="57" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B57" s="8" t="s">
-        <v>159</v>
-      </c>
-      <c r="C57" s="8">
-        <v>1</v>
-      </c>
-      <c r="D57" s="7" t="s">
-        <v>161</v>
-      </c>
-      <c r="E57" s="7" t="s">
-        <v>160</v>
-      </c>
-      <c r="F57" s="7" t="s">
-        <v>162</v>
-      </c>
-      <c r="H57" s="7" t="s">
-        <v>120</v>
-      </c>
-      <c r="J57" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="K57" s="1" t="s">
-        <v>164</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changed power caps to 0805. working on BOM
</commit_message>
<xml_diff>
--- a/CANnode/Output/BOM_Final.xlsx
+++ b/CANnode/Output/BOM_Final.xlsx
@@ -1,16 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="26221"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-30" yWindow="-120" windowWidth="20730" windowHeight="11760"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28780" windowHeight="17540"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
@@ -19,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="227">
   <si>
     <t>Qty</t>
   </si>
@@ -66,24 +69,9 @@
     <t>1K</t>
   </si>
   <si>
-    <t>R98, R99, R100, R101</t>
-  </si>
-  <si>
-    <t>1k</t>
-  </si>
-  <si>
-    <t>R40, R66, R67, R68, R69, R77, R78, R79</t>
-  </si>
-  <si>
     <t>1uF</t>
   </si>
   <si>
-    <t>C11, C12, C29, C30, C31, C36, C37, C38, C39, C40, C41, C42, C47, C48, C49, C50</t>
-  </si>
-  <si>
-    <t>C1, C2</t>
-  </si>
-  <si>
     <t>2.2K</t>
   </si>
   <si>
@@ -129,18 +117,6 @@
     <t>Y1</t>
   </si>
   <si>
-    <t>20.1K</t>
-  </si>
-  <si>
-    <t>R8</t>
-  </si>
-  <si>
-    <t>20.1k</t>
-  </si>
-  <si>
-    <t>R10, R12, R14, R16, R18, R20, R22, R24, R26, R28, R30, R32, R34, R36, R38, R43, R45, R47, R49, R51, R53, R55, R57</t>
-  </si>
-  <si>
     <t>R41, R42</t>
   </si>
   <si>
@@ -174,42 +150,12 @@
     <t>100K</t>
   </si>
   <si>
-    <t>R115</t>
-  </si>
-  <si>
-    <t>100k</t>
-  </si>
-  <si>
-    <t>R7</t>
-  </si>
-  <si>
     <t>100nF</t>
   </si>
   <si>
-    <t>C13, C14, C15, C16, C17, C18, C19, C21, C22, C23, C24, C25, C73, C75</t>
-  </si>
-  <si>
-    <t>C51, C52, C53, C54, C55, C60, C61, C62, C63, C64, C65, C66, C67, C68, C69, C70</t>
-  </si>
-  <si>
-    <t>C6, C74</t>
-  </si>
-  <si>
     <t>120R</t>
   </si>
   <si>
-    <t>R114</t>
-  </si>
-  <si>
-    <t>R96</t>
-  </si>
-  <si>
-    <t>200R</t>
-  </si>
-  <si>
-    <t>R106, R107</t>
-  </si>
-  <si>
     <t>220R @ 100M</t>
   </si>
   <si>
@@ -241,9 +187,6 @@
   </si>
   <si>
     <t>DNP</t>
-  </si>
-  <si>
-    <t>R5, R6, R59</t>
   </si>
   <si>
     <t>FDV302P</t>
@@ -624,29 +567,152 @@
     <t>Murata Electronics North America</t>
   </si>
   <si>
-    <t>C0402C103J4RACTU</t>
-  </si>
-  <si>
-    <t>Kemet</t>
-  </si>
-  <si>
     <t>GRM155R71C104JA88D</t>
   </si>
   <si>
-    <t>RC0402J000CS</t>
-  </si>
-  <si>
     <t>RC0402FR-07100KL</t>
   </si>
   <si>
     <t>Yageo</t>
+  </si>
+  <si>
+    <t>CAP CER 10000PF 50V X7R 0402</t>
+  </si>
+  <si>
+    <t>GRM155R71H103KA88D</t>
+  </si>
+  <si>
+    <t>CAP CER 0.1UF 16V X7R 0402</t>
+  </si>
+  <si>
+    <t>RC0402JR-070RL</t>
+  </si>
+  <si>
+    <t>RES SMD 0.0OHM JUMPER 1/16W 0402</t>
+  </si>
+  <si>
+    <t>RES SMD 100K OHM 1% 1/16W 0402</t>
+  </si>
+  <si>
+    <t>R7, R115</t>
+  </si>
+  <si>
+    <t>C13, C14, C15, C16, C17, C18, C19, C21, C22, C23, C24, C25, C73, C75, C51, C52, C53, C54, C55, C60, C61, C62, C63, C64, C65, C66, C67, C68, C69, C70, C6, C74</t>
+  </si>
+  <si>
+    <t>R40, R66, R67, R68, R69, R77, R78, R79, R98, R99, R100, R101</t>
+  </si>
+  <si>
+    <t>C1, C2,C11, C12, C29, C30, C31, C36, C37, C38, C39, C40, C41, C42, C47, C48, C49, C50</t>
+  </si>
+  <si>
+    <t>R8,R10, R12, R14, R16, R18, R20, R22, R24, R26, R28, R30, R32, R34, R36, R38, R43, R45, R47, R49, R51, R53, R55, R57</t>
+  </si>
+  <si>
+    <t>R96,R106, R107</t>
+  </si>
+  <si>
+    <t>RC0402JR-0710KL</t>
+  </si>
+  <si>
+    <t>RES SMD 10K OHM 5% 1/16W 0402</t>
+  </si>
+  <si>
+    <t>R5,R6,R114</t>
+  </si>
+  <si>
+    <t>R59</t>
+  </si>
+  <si>
+    <t>Vishay Dale</t>
+  </si>
+  <si>
+    <t>CRCW0402120RJNEDHP</t>
+  </si>
+  <si>
+    <t>RES SMD 120 OHM 5% 1/5W 0402</t>
+  </si>
+  <si>
+    <t>RC0402JR-0712KL</t>
+  </si>
+  <si>
+    <t>RES SMD 12K OHM 5% 1/16W 0402</t>
+  </si>
+  <si>
+    <t>RES SMD 1K OHM 1% 1/16W 0402</t>
+  </si>
+  <si>
+    <t>RC0402FR-071KL</t>
+  </si>
+  <si>
+    <t>GRM155R60J105KE19D</t>
+  </si>
+  <si>
+    <t>CAP CER 1UF 6.3V X5R 0402</t>
+  </si>
+  <si>
+    <t>ERJ-2GEJ222X</t>
+  </si>
+  <si>
+    <t>Panasonic Electronic Components</t>
+  </si>
+  <si>
+    <t>RES SMD 2.2K OHM 5% 1/10W 0402</t>
+  </si>
+  <si>
+    <t>20K</t>
+  </si>
+  <si>
+    <t>tol</t>
+  </si>
+  <si>
+    <t>Vhigh</t>
+  </si>
+  <si>
+    <t>Vlow</t>
+  </si>
+  <si>
+    <t>error</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -tol</t>
+  </si>
+  <si>
+    <t>Susumu</t>
+  </si>
+  <si>
+    <t>RR0510P-203-D</t>
+  </si>
+  <si>
+    <t>RES SMD 20K OHM 0.5% 1/16W 0402</t>
+  </si>
+  <si>
+    <t>ERJ-2RKF2000X</t>
+  </si>
+  <si>
+    <t>RES SMD 200 OHM 1% 1/10W 0402</t>
+  </si>
+  <si>
+    <t>RC0402FR-0722RL</t>
+  </si>
+  <si>
+    <t>RES SMD 22 OHM 1% 1/16W 0402</t>
+  </si>
+  <si>
+    <t>500R07S220JV4T</t>
+  </si>
+  <si>
+    <t>Johanson Technology Inc.</t>
+  </si>
+  <si>
+    <t>CAP CER 22PF 50V NP0 0402</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -688,6 +754,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -712,16 +794,16 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -750,11 +832,60 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -788,9 +919,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyAlignment="1">
@@ -804,12 +932,72 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="51">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
+    <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="11" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="13" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="15" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="17" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="19" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="21" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="23" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="25" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="27" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="29" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="31" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="33" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="35" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="37" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="39" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="41" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="43" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="45" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="47" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="49" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="11">
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -824,9 +1012,6 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -858,8 +1043,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:K55" totalsRowShown="0">
-  <autoFilter ref="A1:K55"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:K48" totalsRowShown="0">
+  <autoFilter ref="A1:K48"/>
   <sortState ref="A2:K56">
     <sortCondition ref="J2:J55" customList=".01uF,.1uF,.1uF,0R,0ZCJ0050AF2E,100K,100k,100nF,100nF,100nF,10K,120R,12K,12M,1751316,1K,1k,1uF,1uF,2.2K,20.1K,20.1k,200,200R,22,220R @ 100M,22pF,22uF,250,250k,39K,4.7K,4.7uF,47uF,698,7M-16.000MAAJ-T,93LC56C-I/SN"/>
   </sortState>
@@ -868,13 +1053,13 @@
     <tableColumn id="2" name="Ref Des" dataDxfId="9"/>
     <tableColumn id="3" name="Qty" dataDxfId="8"/>
     <tableColumn id="4" name="Manufacturer" dataDxfId="7"/>
-    <tableColumn id="5" name="Mfg Part #" dataDxfId="6"/>
-    <tableColumn id="6" name="Description" dataDxfId="5"/>
-    <tableColumn id="7" name="Package" dataDxfId="4"/>
-    <tableColumn id="8" name="Type" dataDxfId="3"/>
-    <tableColumn id="9" name="Your Instructions" dataDxfId="2"/>
-    <tableColumn id="12" name="Value" dataDxfId="1"/>
-    <tableColumn id="13" name="Device" dataDxfId="0"/>
+    <tableColumn id="5" name="Mfg Part #" dataDxfId="0"/>
+    <tableColumn id="6" name="Description" dataDxfId="6"/>
+    <tableColumn id="7" name="Package" dataDxfId="5"/>
+    <tableColumn id="8" name="Type" dataDxfId="4"/>
+    <tableColumn id="9" name="Your Instructions" dataDxfId="3"/>
+    <tableColumn id="12" name="Value" dataDxfId="2"/>
+    <tableColumn id="13" name="Device" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1135,7 +1320,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1143,56 +1328,58 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L55"/>
+  <dimension ref="A1:P48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="7"/>
-    <col min="2" max="2" width="37.7109375" style="7" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="7"/>
-    <col min="4" max="4" width="16.42578125" style="7" customWidth="1"/>
-    <col min="5" max="5" width="19.42578125" style="7" customWidth="1"/>
-    <col min="6" max="6" width="22.140625" style="7" customWidth="1"/>
+    <col min="1" max="1" width="8.83203125" style="7"/>
+    <col min="2" max="2" width="37.6640625" style="7" customWidth="1"/>
+    <col min="3" max="3" width="8.83203125" style="7"/>
+    <col min="4" max="4" width="16.5" style="7" customWidth="1"/>
+    <col min="5" max="5" width="19.5" style="12" customWidth="1"/>
+    <col min="6" max="6" width="22.1640625" style="7" customWidth="1"/>
     <col min="7" max="7" width="11" style="12" customWidth="1"/>
-    <col min="8" max="8" width="9.140625" style="7"/>
-    <col min="9" max="9" width="18.140625" style="7" customWidth="1"/>
-    <col min="10" max="10" width="25.42578125" style="6" customWidth="1"/>
-    <col min="11" max="11" width="19.85546875" style="6" customWidth="1"/>
-    <col min="12" max="12" width="40.140625" style="6" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="6"/>
+    <col min="8" max="8" width="8.83203125" style="7"/>
+    <col min="9" max="9" width="18.1640625" style="7" customWidth="1"/>
+    <col min="10" max="10" width="25.5" style="6" customWidth="1"/>
+    <col min="11" max="11" width="19.83203125" style="6" customWidth="1"/>
+    <col min="12" max="12" width="40.1640625" style="6" customWidth="1"/>
+    <col min="13" max="15" width="8.83203125" style="6"/>
+    <col min="16" max="16" width="11" style="6" bestFit="1" customWidth="1"/>
+    <col min="17" max="16384" width="8.83203125" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16">
       <c r="A1" s="3" t="s">
-        <v>94</v>
+        <v>74</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>95</v>
+        <v>75</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>97</v>
+        <v>76</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>77</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>98</v>
+        <v>78</v>
       </c>
       <c r="G1" s="11" t="s">
-        <v>99</v>
+        <v>79</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>101</v>
+        <v>81</v>
       </c>
       <c r="J1" s="2" t="s">
         <v>1</v>
@@ -1201,7 +1388,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16">
       <c r="B2" s="8" t="s">
         <v>7</v>
       </c>
@@ -1209,59 +1396,57 @@
         <v>8</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>201</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>200</v>
-      </c>
-      <c r="F2" s="7" t="str">
-        <f>CONCATENATE(LEFT(Table1[[#This Row],[Device]],3)," ",Table1[[#This Row],[Value]]," ",RIGHT(Table1[[#This Row],[Device]],4))</f>
-        <v>CAP .01uF 0402</v>
+        <v>179</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>184</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>183</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>109</v>
+        <v>89</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>114</v>
+        <v>94</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>6</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16">
       <c r="B3" s="8" t="s">
-        <v>111</v>
+        <v>91</v>
       </c>
       <c r="C3" s="8">
         <v>4</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>199</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>202</v>
-      </c>
-      <c r="F3" s="7" t="str">
-        <f>CONCATENATE(LEFT(Table1[[#This Row],[Device]],3)," ",Table1[[#This Row],[Value]]," ",RIGHT(Table1[[#This Row],[Device]],4))</f>
-        <v>CAP .1uF 0402</v>
+        <v>179</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>180</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>185</v>
       </c>
       <c r="G3" s="12" t="s">
-        <v>109</v>
+        <v>89</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>114</v>
+        <v>94</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>5</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16">
       <c r="B4" s="8" t="s">
         <v>10</v>
       </c>
@@ -1269,20 +1454,19 @@
         <v>11</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>161</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>203</v>
-      </c>
-      <c r="F4" s="7" t="str">
-        <f>CONCATENATE(LEFT(Table1[[#This Row],[Device]],3)," ",Table1[[#This Row],[Value]]," ",RIGHT(Table1[[#This Row],[Device]],4))</f>
-        <v>RES 0R 0402</v>
+        <v>182</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>186</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>187</v>
       </c>
       <c r="G4" s="12" t="s">
-        <v>109</v>
+        <v>89</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>114</v>
+        <v>94</v>
       </c>
       <c r="J4" s="1" t="s">
         <v>8</v>
@@ -1291,7 +1475,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16">
       <c r="B5" s="8" t="s">
         <v>13</v>
       </c>
@@ -1299,19 +1483,19 @@
         <v>1</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="E5" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="E5" s="12" t="s">
         <v>11</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>113</v>
+        <v>93</v>
       </c>
       <c r="G5" s="12" t="s">
-        <v>110</v>
+        <v>90</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>114</v>
+        <v>94</v>
       </c>
       <c r="J5" s="1" t="s">
         <v>11</v>
@@ -1320,906 +1504,1022 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16">
       <c r="B6" s="8" t="s">
-        <v>51</v>
+        <v>189</v>
       </c>
       <c r="C6" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>205</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>204</v>
-      </c>
-      <c r="F6" s="7" t="str">
-        <f>CONCATENATE(LEFT(Table1[[#This Row],[Device]],3)," ",Table1[[#This Row],[Value]]," ",RIGHT(Table1[[#This Row],[Device]],4))</f>
-        <v>RES 100K 0402</v>
+        <v>182</v>
+      </c>
+      <c r="E6" s="12" t="s">
+        <v>181</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>188</v>
       </c>
       <c r="G6" s="12" t="s">
-        <v>109</v>
+        <v>89</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>114</v>
+        <v>94</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="K6" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16">
       <c r="B7" s="8" t="s">
-        <v>53</v>
+        <v>190</v>
       </c>
       <c r="C7" s="8">
-        <v>1</v>
+        <v>32</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>205</v>
-      </c>
-      <c r="E7" s="7" t="s">
-        <v>204</v>
-      </c>
-      <c r="F7" s="7" t="str">
-        <f>CONCATENATE(LEFT(Table1[[#This Row],[Device]],3)," ",Table1[[#This Row],[Value]]," ",RIGHT(Table1[[#This Row],[Device]],4))</f>
-        <v>RES 100k 0402</v>
+        <v>179</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>180</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>185</v>
       </c>
       <c r="G7" s="12" t="s">
-        <v>109</v>
+        <v>89</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>114</v>
+        <v>94</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="K7" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16">
+      <c r="B8" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="8">
+        <v>2</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>195</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>196</v>
+      </c>
+      <c r="G8" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="H8" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K8" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B8" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="C8" s="8">
-        <v>14</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>199</v>
-      </c>
-      <c r="E8" s="7" t="s">
-        <v>202</v>
-      </c>
-      <c r="F8" s="7" t="str">
-        <f>CONCATENATE(LEFT(Table1[[#This Row],[Device]],3)," ",Table1[[#This Row],[Value]]," ",RIGHT(Table1[[#This Row],[Device]],4))</f>
-        <v>CAP 100nF 0402</v>
-      </c>
-      <c r="G8" s="12" t="s">
-        <v>109</v>
-      </c>
-      <c r="H8" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="J8" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="K8" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16">
       <c r="B9" s="8" t="s">
-        <v>56</v>
+        <v>197</v>
       </c>
       <c r="C9" s="8">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="D9" s="7" t="s">
         <v>199</v>
       </c>
-      <c r="E9" s="7" t="s">
+      <c r="E9" s="12" t="s">
+        <v>200</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>201</v>
+      </c>
+      <c r="G9" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="H9" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16">
+      <c r="B10" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" s="8">
+        <v>1</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="E10" s="12" t="s">
         <v>202</v>
       </c>
-      <c r="F9" s="7" t="str">
-        <f>CONCATENATE(LEFT(Table1[[#This Row],[Device]],3)," ",Table1[[#This Row],[Value]]," ",RIGHT(Table1[[#This Row],[Device]],4))</f>
-        <v>CAP 100nF 0402</v>
-      </c>
-      <c r="G9" s="12" t="s">
-        <v>109</v>
-      </c>
-      <c r="H9" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="J9" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="K9" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B10" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="C10" s="8">
-        <v>2</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>199</v>
-      </c>
-      <c r="E10" s="7" t="s">
-        <v>202</v>
-      </c>
-      <c r="F10" s="7" t="str">
-        <f>CONCATENATE(LEFT(Table1[[#This Row],[Device]],3)," ",Table1[[#This Row],[Value]]," ",RIGHT(Table1[[#This Row],[Device]],4))</f>
-        <v>CAP 100nF 0402</v>
+      <c r="F10" s="7" t="s">
+        <v>203</v>
       </c>
       <c r="G10" s="12" t="s">
-        <v>109</v>
+        <v>89</v>
       </c>
       <c r="H10" s="7" t="s">
-        <v>114</v>
+        <v>94</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>54</v>
+        <v>26</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B11" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16">
+      <c r="A11" s="14"/>
+      <c r="B11" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="C11" s="8">
-        <v>2</v>
-      </c>
-      <c r="F11" s="7" t="str">
-        <f>CONCATENATE(LEFT(Table1[[#This Row],[Device]],3)," ",Table1[[#This Row],[Value]]," ",RIGHT(Table1[[#This Row],[Device]],4))</f>
-        <v>RES 10K 0402</v>
-      </c>
-      <c r="G11" s="12" t="s">
-        <v>109</v>
-      </c>
-      <c r="H11" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="J11" s="1" t="s">
+      <c r="C11" s="15">
+        <v>1</v>
+      </c>
+      <c r="D11" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="E11" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="F11" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="G11" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="H11" s="14"/>
+      <c r="I11" s="14"/>
+      <c r="J11" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="K11" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="K11" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:16">
       <c r="B12" s="8" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="C12" s="8">
         <v>1</v>
       </c>
-      <c r="F12" s="7" t="str">
-        <f>CONCATENATE(LEFT(Table1[[#This Row],[Device]],3)," ",Table1[[#This Row],[Value]]," ",RIGHT(Table1[[#This Row],[Device]],4))</f>
-        <v>RES 120R 0402</v>
+      <c r="D12" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="E12" s="20">
+        <v>1751316</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>100</v>
       </c>
       <c r="G12" s="12" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="H12" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="J12" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="K12" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+      <c r="J12" s="18">
+        <v>1751316</v>
+      </c>
+      <c r="K12" s="18">
+        <v>1751316</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16">
       <c r="B13" s="8" t="s">
-        <v>32</v>
+        <v>191</v>
       </c>
       <c r="C13" s="8">
-        <v>1</v>
-      </c>
-      <c r="F13" s="7" t="str">
-        <f>CONCATENATE(LEFT(Table1[[#This Row],[Device]],3)," ",Table1[[#This Row],[Value]]," ",RIGHT(Table1[[#This Row],[Device]],4))</f>
-        <v>RES 12K 0402</v>
+        <v>12</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="E13" s="12" t="s">
+        <v>205</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>204</v>
       </c>
       <c r="G13" s="12" t="s">
-        <v>109</v>
+        <v>89</v>
       </c>
       <c r="H13" s="7" t="s">
-        <v>114</v>
+        <v>94</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>31</v>
+        <v>14</v>
       </c>
       <c r="K13" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="15"/>
-      <c r="B14" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="C14" s="16">
-        <v>1</v>
-      </c>
-      <c r="D14" s="15" t="s">
-        <v>116</v>
-      </c>
-      <c r="E14" s="15" t="s">
-        <v>115</v>
-      </c>
-      <c r="F14" s="15" t="s">
-        <v>117</v>
-      </c>
-      <c r="G14" s="17" t="s">
-        <v>118</v>
-      </c>
-      <c r="H14" s="15"/>
-      <c r="I14" s="15"/>
-      <c r="J14" s="18" t="s">
+    <row r="14" spans="1:16">
+      <c r="B14" s="8" t="s">
+        <v>192</v>
+      </c>
+      <c r="C14" s="8">
+        <v>18</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="E14" s="12" t="s">
+        <v>206</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="G14" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="H14" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K14" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="K14" s="18" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:16">
       <c r="B15" s="8" t="s">
-        <v>70</v>
+        <v>17</v>
       </c>
       <c r="C15" s="8">
         <v>1</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="E15" s="13">
-        <v>1751316</v>
+        <v>209</v>
+      </c>
+      <c r="E15" s="12" t="s">
+        <v>208</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>120</v>
+        <v>210</v>
       </c>
       <c r="G15" s="12" t="s">
-        <v>122</v>
+        <v>89</v>
       </c>
       <c r="H15" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="J15" s="19">
-        <v>1751316</v>
-      </c>
-      <c r="K15" s="19">
-        <v>1751316</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L15" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="M15" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="N15" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="O15" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="P15" s="6" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16">
       <c r="B16" s="8" t="s">
-        <v>15</v>
+        <v>193</v>
       </c>
       <c r="C16" s="8">
-        <v>4</v>
-      </c>
-      <c r="F16" s="7" t="str">
-        <f>CONCATENATE(LEFT(Table1[[#This Row],[Device]],3)," ",Table1[[#This Row],[Value]]," ",RIGHT(Table1[[#This Row],[Device]],4))</f>
-        <v>RES 1K 0402</v>
+        <v>24</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>217</v>
+      </c>
+      <c r="E16" s="12" t="s">
+        <v>218</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>219</v>
       </c>
       <c r="G16" s="12" t="s">
-        <v>109</v>
+        <v>89</v>
       </c>
       <c r="H16" s="7" t="s">
-        <v>114</v>
+        <v>94</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>14</v>
+        <v>211</v>
       </c>
       <c r="K16" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="L16" s="6">
+        <f>39*(1-N16)/(39*(1-N16)+20*(1+N16))*5</f>
+        <v>3.2826049991498039</v>
+      </c>
+      <c r="M16" s="6">
+        <f>39*(1-O16)/(39*(1-O16)+20*(1+O16))*5</f>
+        <v>3.327420172326407</v>
+      </c>
+      <c r="N16" s="6">
+        <v>0.01</v>
+      </c>
+      <c r="O16" s="6">
+        <v>-0.01</v>
+      </c>
+      <c r="P16" s="6">
+        <f>(M16-L16)/3.3*100</f>
+        <v>1.3580355508061548</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16">
       <c r="B17" s="8" t="s">
-        <v>17</v>
+        <v>194</v>
       </c>
       <c r="C17" s="8">
-        <v>8</v>
-      </c>
-      <c r="F17" s="7" t="str">
-        <f>CONCATENATE(LEFT(Table1[[#This Row],[Device]],3)," ",Table1[[#This Row],[Value]]," ",RIGHT(Table1[[#This Row],[Device]],4))</f>
-        <v>RES 1k 0402</v>
+        <v>3</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>209</v>
+      </c>
+      <c r="E17" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>221</v>
       </c>
       <c r="G17" s="12" t="s">
-        <v>109</v>
+        <v>89</v>
       </c>
       <c r="H17" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="J17" s="1" t="s">
-        <v>16</v>
+        <v>94</v>
+      </c>
+      <c r="J17" s="1">
+        <v>200</v>
       </c>
       <c r="K17" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="L17" s="6">
+        <f>39*(1-N17)/(39*(1-N17)+20*(1+N17))*5</f>
+        <v>3.302843288516641</v>
+      </c>
+      <c r="M17" s="6">
+        <f>39*(1-O17)/(39*(1-O17)+20*(1+O17))*5</f>
+        <v>3.3073247598231075</v>
+      </c>
+      <c r="N17" s="6">
+        <v>1E-3</v>
+      </c>
+      <c r="O17" s="6">
+        <v>-1E-3</v>
+      </c>
+      <c r="P17" s="6">
+        <f>(M17-L17)/3.3*100</f>
+        <v>0.13580216080201449</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16">
       <c r="B18" s="8" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="C18" s="8">
-        <v>16</v>
-      </c>
-      <c r="F18" s="7" t="str">
-        <f>CONCATENATE(LEFT(Table1[[#This Row],[Device]],3)," ",Table1[[#This Row],[Value]]," ",RIGHT(Table1[[#This Row],[Device]],4))</f>
-        <v>CAP 1uF 0402</v>
+        <v>2</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="E18" s="12" t="s">
+        <v>222</v>
+      </c>
+      <c r="F18" s="7" t="s">
+        <v>223</v>
       </c>
       <c r="G18" s="12" t="s">
-        <v>109</v>
+        <v>89</v>
       </c>
       <c r="H18" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="J18" s="1" t="s">
-        <v>18</v>
+        <v>94</v>
+      </c>
+      <c r="J18" s="1">
+        <v>22</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16">
       <c r="B19" s="8" t="s">
-        <v>20</v>
+        <v>46</v>
       </c>
       <c r="C19" s="8">
         <v>2</v>
       </c>
-      <c r="F19" s="7" t="str">
-        <f>CONCATENATE(LEFT(Table1[[#This Row],[Device]],3)," ",Table1[[#This Row],[Value]]," ",RIGHT(Table1[[#This Row],[Device]],4))</f>
-        <v>CAP 1uF 0402</v>
+      <c r="D19" t="s">
+        <v>87</v>
+      </c>
+      <c r="E19" s="21" t="s">
+        <v>86</v>
+      </c>
+      <c r="F19" t="s">
+        <v>85</v>
       </c>
       <c r="G19" s="12" t="s">
-        <v>109</v>
+        <v>88</v>
       </c>
       <c r="H19" s="7" t="s">
-        <v>114</v>
+        <v>94</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>18</v>
+        <v>44</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16">
       <c r="B20" s="8" t="s">
-        <v>22</v>
+        <v>83</v>
       </c>
       <c r="C20" s="8">
-        <v>1</v>
-      </c>
-      <c r="F20" s="7" t="str">
-        <f>CONCATENATE(LEFT(Table1[[#This Row],[Device]],3)," ",Table1[[#This Row],[Value]]," ",RIGHT(Table1[[#This Row],[Device]],4))</f>
-        <v>RES 2.2K 0402</v>
+        <v>4</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>225</v>
+      </c>
+      <c r="E20" s="12" t="s">
+        <v>224</v>
+      </c>
+      <c r="F20" s="7" t="s">
+        <v>226</v>
       </c>
       <c r="G20" s="12" t="s">
-        <v>109</v>
+        <v>89</v>
       </c>
       <c r="H20" s="7" t="s">
-        <v>114</v>
+        <v>94</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16">
       <c r="B21" s="8" t="s">
-        <v>37</v>
+        <v>84</v>
       </c>
       <c r="C21" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F21" s="7" t="str">
         <f>CONCATENATE(LEFT(Table1[[#This Row],[Device]],3)," ",Table1[[#This Row],[Value]]," ",RIGHT(Table1[[#This Row],[Device]],4))</f>
-        <v>RES 20.1K 0402</v>
+        <v>CAP 22uF 0402</v>
       </c>
       <c r="G21" s="12" t="s">
-        <v>109</v>
+        <v>89</v>
       </c>
       <c r="H21" s="7" t="s">
-        <v>114</v>
+        <v>94</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="K21" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16">
       <c r="B22" s="8" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="C22" s="8">
-        <v>23</v>
-      </c>
-      <c r="F22" s="7" t="str">
-        <f>CONCATENATE(LEFT(Table1[[#This Row],[Device]],3)," ",Table1[[#This Row],[Value]]," ",RIGHT(Table1[[#This Row],[Device]],4))</f>
-        <v>RES 20.1k 0402</v>
+        <v>1</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="E22" s="12" t="s">
+        <v>143</v>
+      </c>
+      <c r="F22" s="7" t="s">
+        <v>142</v>
       </c>
       <c r="G22" s="12" t="s">
-        <v>109</v>
+        <v>89</v>
       </c>
       <c r="H22" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="J22" s="1" t="s">
-        <v>38</v>
+        <v>94</v>
+      </c>
+      <c r="J22" s="1">
+        <v>619</v>
       </c>
       <c r="K22" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16">
       <c r="B23" s="8" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="C23" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F23" s="7" t="str">
         <f>CONCATENATE(LEFT(Table1[[#This Row],[Device]],3)," ",Table1[[#This Row],[Value]]," ",RIGHT(Table1[[#This Row],[Device]],4))</f>
-        <v>RES 200 0402</v>
+        <v>RES 250k 0402</v>
       </c>
       <c r="G23" s="12" t="s">
-        <v>109</v>
+        <v>89</v>
       </c>
       <c r="H23" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="J23" s="1">
-        <v>200</v>
+        <v>94</v>
+      </c>
+      <c r="J23" s="1" t="s">
+        <v>48</v>
       </c>
       <c r="K23" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16">
       <c r="B24" s="8" t="s">
-        <v>62</v>
+        <v>36</v>
       </c>
       <c r="C24" s="8">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="F24" s="7" t="str">
         <f>CONCATENATE(LEFT(Table1[[#This Row],[Device]],3)," ",Table1[[#This Row],[Value]]," ",RIGHT(Table1[[#This Row],[Device]],4))</f>
-        <v>RES 200R 0402</v>
+        <v>RES 39K 0402</v>
       </c>
       <c r="G24" s="12" t="s">
-        <v>109</v>
+        <v>89</v>
       </c>
       <c r="H24" s="7" t="s">
-        <v>114</v>
+        <v>94</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>61</v>
+        <v>35</v>
       </c>
       <c r="K24" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16">
       <c r="B25" s="8" t="s">
-        <v>40</v>
+        <v>19</v>
       </c>
       <c r="C25" s="8">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F25" s="7" t="str">
         <f>CONCATENATE(LEFT(Table1[[#This Row],[Device]],3)," ",Table1[[#This Row],[Value]]," ",RIGHT(Table1[[#This Row],[Device]],4))</f>
-        <v>RES 22 0402</v>
+        <v>RES 4.7K 0402</v>
       </c>
       <c r="G25" s="12" t="s">
-        <v>109</v>
+        <v>89</v>
       </c>
       <c r="H25" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="J25" s="1">
-        <v>22</v>
+        <v>94</v>
+      </c>
+      <c r="J25" s="1" t="s">
+        <v>18</v>
       </c>
       <c r="K25" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16">
       <c r="B26" s="8" t="s">
-        <v>65</v>
+        <v>82</v>
       </c>
       <c r="C26" s="8">
-        <v>2</v>
-      </c>
-      <c r="D26" t="s">
-        <v>107</v>
-      </c>
-      <c r="E26" t="s">
-        <v>106</v>
-      </c>
-      <c r="F26" t="s">
-        <v>105</v>
+        <v>7</v>
+      </c>
+      <c r="F26" s="7" t="str">
+        <f>CONCATENATE(LEFT(Table1[[#This Row],[Device]],3)," ",Table1[[#This Row],[Value]]," ",RIGHT(Table1[[#This Row],[Device]],4))</f>
+        <v>CAP 4.7uF 0805</v>
       </c>
       <c r="G26" s="12" t="s">
-        <v>108</v>
+        <v>88</v>
       </c>
       <c r="H26" s="7" t="s">
-        <v>114</v>
+        <v>94</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>63</v>
+        <v>20</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="27" spans="2:11" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16">
       <c r="B27" s="8" t="s">
-        <v>103</v>
+        <v>38</v>
       </c>
       <c r="C27" s="8">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F27" s="7" t="str">
         <f>CONCATENATE(LEFT(Table1[[#This Row],[Device]],3)," ",Table1[[#This Row],[Value]]," ",RIGHT(Table1[[#This Row],[Device]],4))</f>
-        <v>CAP 22pF 0402</v>
+        <v>CAP 47uF 0402</v>
       </c>
       <c r="G27" s="12" t="s">
-        <v>109</v>
+        <v>89</v>
       </c>
       <c r="H27" s="7" t="s">
-        <v>114</v>
+        <v>94</v>
       </c>
       <c r="J27" s="1" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="K27" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="28" spans="2:11" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16">
       <c r="B28" s="8" t="s">
-        <v>104</v>
+        <v>50</v>
       </c>
       <c r="C28" s="8">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="F28" s="7" t="str">
         <f>CONCATENATE(LEFT(Table1[[#This Row],[Device]],3)," ",Table1[[#This Row],[Value]]," ",RIGHT(Table1[[#This Row],[Device]],4))</f>
-        <v>CAP 22uF 0402</v>
+        <v>RES 698 0402</v>
       </c>
       <c r="G28" s="12" t="s">
-        <v>109</v>
+        <v>89</v>
       </c>
       <c r="H28" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="J28" s="1" t="s">
-        <v>43</v>
+        <v>94</v>
+      </c>
+      <c r="J28" s="1">
+        <v>698</v>
       </c>
       <c r="K28" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="29" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B29" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="C29" s="8">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16">
+      <c r="A29" s="14"/>
+      <c r="B29" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="C29" s="15">
         <v>1</v>
       </c>
-      <c r="D29" s="7" t="s">
-        <v>161</v>
-      </c>
-      <c r="E29" s="7" t="s">
-        <v>163</v>
-      </c>
-      <c r="F29" s="7" t="s">
-        <v>162</v>
-      </c>
-      <c r="G29" s="12" t="s">
-        <v>109</v>
-      </c>
-      <c r="H29" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="J29" s="1">
-        <v>619</v>
-      </c>
-      <c r="K29" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="30" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="D29" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="E29" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="F29" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="G29" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="H29" s="14"/>
+      <c r="I29" s="14"/>
+      <c r="J29" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="K29" s="17" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16">
       <c r="B30" s="8" t="s">
-        <v>68</v>
+        <v>40</v>
       </c>
       <c r="C30" s="8">
-        <v>2</v>
-      </c>
-      <c r="F30" s="7" t="str">
-        <f>CONCATENATE(LEFT(Table1[[#This Row],[Device]],3)," ",Table1[[#This Row],[Value]]," ",RIGHT(Table1[[#This Row],[Device]],4))</f>
-        <v>RES 250k 0402</v>
+        <v>1</v>
+      </c>
+      <c r="D30" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="E30" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="F30" s="7" t="s">
+        <v>150</v>
       </c>
       <c r="G30" s="12" t="s">
-        <v>109</v>
+        <v>151</v>
       </c>
       <c r="H30" s="7" t="s">
-        <v>114</v>
+        <v>94</v>
       </c>
       <c r="J30" s="1" t="s">
-        <v>67</v>
+        <v>39</v>
       </c>
       <c r="K30" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="31" spans="2:11" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16">
       <c r="B31" s="8" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="C31" s="8">
-        <v>25</v>
-      </c>
-      <c r="F31" s="7" t="str">
-        <f>CONCATENATE(LEFT(Table1[[#This Row],[Device]],3)," ",Table1[[#This Row],[Value]]," ",RIGHT(Table1[[#This Row],[Device]],4))</f>
-        <v>RES 39K 0402</v>
-      </c>
-      <c r="G31" s="12" t="s">
-        <v>109</v>
-      </c>
-      <c r="H31" s="7" t="s">
-        <v>114</v>
+        <v>1</v>
+      </c>
+      <c r="D31" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="E31" s="12" t="s">
+        <v>172</v>
+      </c>
+      <c r="F31" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="I31" s="7" t="s">
+        <v>174</v>
       </c>
       <c r="J31" s="1" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="K31" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="32" spans="2:11" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16">
       <c r="B32" s="8" t="s">
-        <v>24</v>
+        <v>198</v>
       </c>
       <c r="C32" s="8">
-        <v>4</v>
-      </c>
-      <c r="F32" s="7" t="str">
-        <f>CONCATENATE(LEFT(Table1[[#This Row],[Device]],3)," ",Table1[[#This Row],[Value]]," ",RIGHT(Table1[[#This Row],[Device]],4))</f>
-        <v>RES 4.7K 0402</v>
-      </c>
-      <c r="G32" s="12" t="s">
-        <v>109</v>
-      </c>
-      <c r="H32" s="7" t="s">
-        <v>114</v>
+        <v>1</v>
       </c>
       <c r="J32" s="1" t="s">
-        <v>23</v>
+        <v>54</v>
       </c>
       <c r="K32" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:12">
       <c r="B33" s="8" t="s">
-        <v>102</v>
+        <v>57</v>
       </c>
       <c r="C33" s="8">
-        <v>7</v>
-      </c>
-      <c r="F33" s="7" t="str">
-        <f>CONCATENATE(LEFT(Table1[[#This Row],[Device]],3)," ",Table1[[#This Row],[Value]]," ",RIGHT(Table1[[#This Row],[Device]],4))</f>
-        <v>CAP 4.7uF 0805</v>
+        <v>2</v>
+      </c>
+      <c r="D33" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="E33" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="F33" s="7" t="s">
+        <v>153</v>
       </c>
       <c r="G33" s="12" t="s">
-        <v>108</v>
+        <v>154</v>
       </c>
       <c r="H33" s="7" t="s">
-        <v>114</v>
+        <v>94</v>
       </c>
       <c r="J33" s="1" t="s">
-        <v>25</v>
+        <v>55</v>
       </c>
       <c r="K33" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="34" spans="2:12">
       <c r="B34" s="8" t="s">
-        <v>47</v>
+        <v>59</v>
       </c>
       <c r="C34" s="8">
         <v>1</v>
       </c>
-      <c r="F34" s="7" t="str">
-        <f>CONCATENATE(LEFT(Table1[[#This Row],[Device]],3)," ",Table1[[#This Row],[Value]]," ",RIGHT(Table1[[#This Row],[Device]],4))</f>
-        <v>CAP 47uF 0402</v>
+      <c r="D34" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="E34" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="F34" s="7" t="s">
+        <v>156</v>
       </c>
       <c r="G34" s="12" t="s">
-        <v>109</v>
+        <v>157</v>
       </c>
       <c r="H34" s="7" t="s">
-        <v>114</v>
+        <v>94</v>
       </c>
       <c r="J34" s="1" t="s">
-        <v>46</v>
+        <v>58</v>
       </c>
       <c r="K34" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="35" spans="2:12">
       <c r="B35" s="8" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="C35" s="8">
-        <v>16</v>
-      </c>
-      <c r="F35" s="7" t="str">
-        <f>CONCATENATE(LEFT(Table1[[#This Row],[Device]],3)," ",Table1[[#This Row],[Value]]," ",RIGHT(Table1[[#This Row],[Device]],4))</f>
-        <v>RES 698 0402</v>
+        <v>2</v>
+      </c>
+      <c r="D35" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="E35" s="12" t="s">
+        <v>160</v>
+      </c>
+      <c r="F35" s="7" t="s">
+        <v>158</v>
       </c>
       <c r="G35" s="12" t="s">
-        <v>109</v>
+        <v>159</v>
       </c>
       <c r="H35" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="J35" s="1">
-        <v>698</v>
+        <v>94</v>
+      </c>
+      <c r="J35" s="1" t="s">
+        <v>60</v>
       </c>
       <c r="K35" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A36" s="15"/>
-      <c r="B36" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="C36" s="16">
-        <v>1</v>
-      </c>
-      <c r="D36" s="15" t="s">
-        <v>116</v>
-      </c>
-      <c r="E36" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="F36" s="15" t="s">
-        <v>117</v>
-      </c>
-      <c r="G36" s="17" t="s">
-        <v>118</v>
-      </c>
-      <c r="H36" s="15"/>
-      <c r="I36" s="15"/>
-      <c r="J36" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="K36" s="18" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="36" spans="2:12">
+      <c r="B36" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="C36" s="8">
+        <v>6</v>
+      </c>
+      <c r="D36" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="E36" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="F36" s="7" t="s">
+        <v>162</v>
+      </c>
+      <c r="G36" s="12" t="s">
+        <v>163</v>
+      </c>
+      <c r="H36" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="J36" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="K36" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="37" spans="2:12" ht="28">
       <c r="B37" s="8" t="s">
-        <v>49</v>
+        <v>65</v>
       </c>
       <c r="C37" s="8">
         <v>1</v>
       </c>
       <c r="D37" s="7" t="s">
-        <v>169</v>
-      </c>
-      <c r="E37" s="7" t="s">
-        <v>48</v>
+        <v>161</v>
+      </c>
+      <c r="E37" s="12" t="s">
+        <v>164</v>
       </c>
       <c r="F37" s="7" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="G37" s="12" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="H37" s="7" t="s">
-        <v>114</v>
+        <v>94</v>
       </c>
       <c r="J37" s="1" t="s">
-        <v>48</v>
+        <v>64</v>
       </c>
       <c r="K37" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="38" spans="2:12">
       <c r="B38" s="8" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="C38" s="8">
         <v>1</v>
       </c>
       <c r="D38" s="7" t="s">
-        <v>193</v>
-      </c>
-      <c r="E38" s="7" t="s">
-        <v>192</v>
-      </c>
-      <c r="F38" s="7" t="s">
-        <v>191</v>
-      </c>
-      <c r="I38" s="7" t="s">
-        <v>194</v>
+        <v>161</v>
+      </c>
+      <c r="E38" s="12" t="s">
+        <v>167</v>
+      </c>
+      <c r="F38" s="13" t="s">
+        <v>168</v>
+      </c>
+      <c r="G38" s="12" t="s">
+        <v>169</v>
+      </c>
+      <c r="H38" s="7" t="s">
+        <v>94</v>
       </c>
       <c r="J38" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="K38" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="39" spans="2:12">
+      <c r="B39" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="C39" s="8">
+        <v>30</v>
+      </c>
+      <c r="D39" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="E39" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="F39" s="19" t="s">
+        <v>124</v>
+      </c>
+      <c r="G39" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="H39" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="J39" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="K39" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="40" spans="2:12" ht="28">
+      <c r="B40" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="K38" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B39" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="C39" s="8">
-        <v>3</v>
-      </c>
-      <c r="J39" s="1" t="s">
+      <c r="C40" s="8">
+        <v>1</v>
+      </c>
+      <c r="D40" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="E40" s="12">
+        <v>1050170001</v>
+      </c>
+      <c r="F40" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="G40" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="H40" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="J40" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="K40" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="41" spans="2:12">
+      <c r="B41" s="8" t="s">
         <v>73</v>
-      </c>
-      <c r="K39" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B40" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="C40" s="8">
-        <v>2</v>
-      </c>
-      <c r="D40" s="7" t="s">
-        <v>172</v>
-      </c>
-      <c r="E40" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="F40" s="7" t="s">
-        <v>173</v>
-      </c>
-      <c r="G40" s="12" t="s">
-        <v>174</v>
-      </c>
-      <c r="H40" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="J40" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="K40" s="1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B41" s="8" t="s">
-        <v>79</v>
       </c>
       <c r="C41" s="8">
         <v>1</v>
@@ -2227,8 +2527,8 @@
       <c r="D41" s="7" t="s">
         <v>175</v>
       </c>
-      <c r="E41" s="1" t="s">
-        <v>78</v>
+      <c r="E41" s="12" t="s">
+        <v>72</v>
       </c>
       <c r="F41" s="7" t="s">
         <v>176</v>
@@ -2237,423 +2537,225 @@
         <v>177</v>
       </c>
       <c r="H41" s="7" t="s">
-        <v>114</v>
+        <v>94</v>
       </c>
       <c r="J41" s="1" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="K41" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+      <c r="L41" s="6" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="42" spans="2:12">
       <c r="B42" s="8" t="s">
-        <v>81</v>
+        <v>170</v>
       </c>
       <c r="C42" s="8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D42" s="7" t="s">
-        <v>181</v>
-      </c>
-      <c r="E42" s="7" t="s">
-        <v>180</v>
+        <v>108</v>
+      </c>
+      <c r="E42" s="12" t="s">
+        <v>113</v>
       </c>
       <c r="F42" s="7" t="s">
-        <v>178</v>
+        <v>112</v>
       </c>
       <c r="G42" s="12" t="s">
-        <v>179</v>
+        <v>88</v>
       </c>
       <c r="H42" s="7" t="s">
-        <v>114</v>
+        <v>94</v>
       </c>
       <c r="J42" s="1" t="s">
-        <v>80</v>
+        <v>110</v>
       </c>
       <c r="K42" s="1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="43" spans="2:12">
       <c r="B43" s="8" t="s">
-        <v>83</v>
+        <v>104</v>
       </c>
       <c r="C43" s="8">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D43" s="7" t="s">
-        <v>181</v>
-      </c>
-      <c r="E43" s="1" t="s">
-        <v>82</v>
+        <v>108</v>
+      </c>
+      <c r="E43" s="12" t="s">
+        <v>107</v>
       </c>
       <c r="F43" s="7" t="s">
-        <v>182</v>
+        <v>109</v>
       </c>
       <c r="G43" s="12" t="s">
-        <v>183</v>
+        <v>88</v>
       </c>
       <c r="H43" s="7" t="s">
-        <v>114</v>
+        <v>94</v>
       </c>
       <c r="J43" s="1" t="s">
-        <v>82</v>
+        <v>111</v>
       </c>
       <c r="K43" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="44" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="44" spans="2:12">
       <c r="B44" s="8" t="s">
-        <v>85</v>
+        <v>103</v>
       </c>
       <c r="C44" s="8">
         <v>1</v>
       </c>
       <c r="D44" s="7" t="s">
-        <v>181</v>
-      </c>
-      <c r="E44" s="7" t="s">
-        <v>184</v>
+        <v>117</v>
+      </c>
+      <c r="E44" s="12" t="s">
+        <v>116</v>
       </c>
       <c r="F44" s="7" t="s">
-        <v>185</v>
+        <v>118</v>
       </c>
       <c r="G44" s="12" t="s">
-        <v>186</v>
+        <v>88</v>
       </c>
       <c r="H44" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="J44" s="9" t="s">
         <v>114</v>
       </c>
-      <c r="J44" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="K44" s="1" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K44" s="10" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="45" spans="2:12">
       <c r="B45" s="8" t="s">
-        <v>87</v>
+        <v>4</v>
       </c>
       <c r="C45" s="8">
         <v>1</v>
       </c>
       <c r="D45" s="7" t="s">
-        <v>181</v>
-      </c>
-      <c r="E45" s="7" t="s">
-        <v>187</v>
-      </c>
-      <c r="F45" s="14" t="s">
-        <v>188</v>
+        <v>146</v>
+      </c>
+      <c r="E45" s="12" t="s">
+        <v>144</v>
+      </c>
+      <c r="F45" s="7" t="s">
+        <v>145</v>
       </c>
       <c r="G45" s="12" t="s">
-        <v>189</v>
+        <v>147</v>
       </c>
       <c r="H45" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="J45" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="K45" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="46" spans="2:12">
+      <c r="B46" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="C46" s="8">
+        <v>1</v>
+      </c>
+      <c r="D46" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="E46" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="F46" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="G46" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="H46" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="J46" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="J45" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="K45" s="1" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B46" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="C46" s="8">
-        <v>30</v>
-      </c>
-      <c r="D46" s="7" t="s">
-        <v>143</v>
-      </c>
-      <c r="E46" s="7" t="s">
-        <v>142</v>
-      </c>
-      <c r="F46" s="20" t="s">
-        <v>144</v>
-      </c>
-      <c r="G46" s="12" t="s">
-        <v>109</v>
-      </c>
-      <c r="H46" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="J46" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="K46" s="1" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="47" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="K46" s="10" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="47" spans="2:12">
       <c r="B47" s="8" t="s">
-        <v>91</v>
+        <v>126</v>
       </c>
       <c r="C47" s="8">
         <v>1</v>
       </c>
       <c r="D47" s="7" t="s">
-        <v>139</v>
-      </c>
-      <c r="E47" s="7">
-        <v>1050170001</v>
+        <v>128</v>
+      </c>
+      <c r="E47" s="12" t="s">
+        <v>129</v>
       </c>
       <c r="F47" s="7" t="s">
-        <v>140</v>
-      </c>
-      <c r="G47" s="12" t="s">
-        <v>141</v>
+        <v>127</v>
       </c>
       <c r="H47" s="7" t="s">
-        <v>114</v>
+        <v>94</v>
       </c>
       <c r="J47" s="1" t="s">
-        <v>90</v>
+        <v>131</v>
       </c>
       <c r="K47" s="1" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="48" spans="2:12">
       <c r="B48" s="8" t="s">
-        <v>93</v>
+        <v>132</v>
       </c>
       <c r="C48" s="8">
         <v>1</v>
       </c>
       <c r="D48" s="7" t="s">
-        <v>195</v>
-      </c>
-      <c r="E48" s="7" t="s">
-        <v>92</v>
+        <v>134</v>
+      </c>
+      <c r="E48" s="12" t="s">
+        <v>133</v>
       </c>
       <c r="F48" s="7" t="s">
-        <v>196</v>
-      </c>
-      <c r="G48" s="12" t="s">
-        <v>197</v>
+        <v>135</v>
       </c>
       <c r="H48" s="7" t="s">
-        <v>114</v>
+        <v>94</v>
       </c>
       <c r="J48" s="1" t="s">
-        <v>92</v>
+        <v>136</v>
       </c>
       <c r="K48" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="L48" s="6" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="49" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B49" s="8" t="s">
-        <v>190</v>
-      </c>
-      <c r="C49" s="8">
-        <v>1</v>
-      </c>
-      <c r="D49" s="7" t="s">
-        <v>128</v>
-      </c>
-      <c r="E49" s="7" t="s">
-        <v>133</v>
-      </c>
-      <c r="F49" s="7" t="s">
-        <v>132</v>
-      </c>
-      <c r="G49" s="12" t="s">
-        <v>108</v>
-      </c>
-      <c r="H49" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="J49" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="K49" s="1" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="50" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B50" s="8" t="s">
-        <v>124</v>
-      </c>
-      <c r="C50" s="8">
-        <v>1</v>
-      </c>
-      <c r="D50" s="7" t="s">
-        <v>128</v>
-      </c>
-      <c r="E50" s="7" t="s">
-        <v>127</v>
-      </c>
-      <c r="F50" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="G50" s="12" t="s">
-        <v>108</v>
-      </c>
-      <c r="H50" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="J50" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="K50" s="1" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="51" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B51" s="8" t="s">
-        <v>123</v>
-      </c>
-      <c r="C51" s="8">
-        <v>1</v>
-      </c>
-      <c r="D51" s="7" t="s">
         <v>137</v>
-      </c>
-      <c r="E51" s="7" t="s">
-        <v>136</v>
-      </c>
-      <c r="F51" s="7" t="s">
-        <v>138</v>
-      </c>
-      <c r="G51" s="12" t="s">
-        <v>108</v>
-      </c>
-      <c r="H51" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="J51" s="9" t="s">
-        <v>134</v>
-      </c>
-      <c r="K51" s="10" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="52" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B52" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C52" s="8">
-        <v>1</v>
-      </c>
-      <c r="D52" s="7" t="s">
-        <v>166</v>
-      </c>
-      <c r="E52" s="7" t="s">
-        <v>164</v>
-      </c>
-      <c r="F52" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="G52" s="12" t="s">
-        <v>167</v>
-      </c>
-      <c r="H52" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="J52" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="K52" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="53" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B53" s="8" t="s">
-        <v>158</v>
-      </c>
-      <c r="C53" s="8">
-        <v>1</v>
-      </c>
-      <c r="D53" s="7" t="s">
-        <v>137</v>
-      </c>
-      <c r="E53" s="7" t="s">
-        <v>159</v>
-      </c>
-      <c r="F53" s="7" t="s">
-        <v>160</v>
-      </c>
-      <c r="G53" s="12" t="s">
-        <v>109</v>
-      </c>
-      <c r="H53" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="J53" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="K53" s="10" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="54" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B54" s="8" t="s">
-        <v>146</v>
-      </c>
-      <c r="C54" s="8">
-        <v>1</v>
-      </c>
-      <c r="D54" s="7" t="s">
-        <v>148</v>
-      </c>
-      <c r="E54" s="7" t="s">
-        <v>149</v>
-      </c>
-      <c r="F54" s="7" t="s">
-        <v>147</v>
-      </c>
-      <c r="H54" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="J54" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="K54" s="1" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="55" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B55" s="8" t="s">
-        <v>152</v>
-      </c>
-      <c r="C55" s="8">
-        <v>1</v>
-      </c>
-      <c r="D55" s="7" t="s">
-        <v>154</v>
-      </c>
-      <c r="E55" s="7" t="s">
-        <v>153</v>
-      </c>
-      <c r="F55" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="H55" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="J55" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="K55" s="1" t="s">
-        <v>157</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId1"/>
   </tableParts>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Revert "Revert "Submittable BOM""
This reverts commit ef0a1a6dea697aed33fd8ed38d90974a342e9a82.
</commit_message>
<xml_diff>
--- a/CANnode/Output/BOM_Final.xlsx
+++ b/CANnode/Output/BOM_Final.xlsx
@@ -1,28 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="26221"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\W2016\Desktop\RM42-CAN-Sensor-Node\CANnode\Output\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28780" windowHeight="17540"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28785" windowHeight="17535"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="238">
   <si>
     <t>Qty</t>
   </si>
@@ -54,9 +59,6 @@
     <t>RES0402</t>
   </si>
   <si>
-    <t>R86, R89, R90, R91, R92, R93, R94, R95, R103, R104, R105</t>
-  </si>
-  <si>
     <t>0ZCJ0050AF2E</t>
   </si>
   <si>
@@ -184,9 +186,6 @@
   </si>
   <si>
     <t>X1</t>
-  </si>
-  <si>
-    <t>DNP</t>
   </si>
   <si>
     <t>FDV302P</t>
@@ -621,9 +620,6 @@
     <t>R5,R6,R114</t>
   </si>
   <si>
-    <t>R59</t>
-  </si>
-  <si>
     <t>Vishay Dale</t>
   </si>
   <si>
@@ -745,6 +741,9 @@
   </si>
   <si>
     <t>Crystal 16MHZ</t>
+  </si>
+  <si>
+    <t>R59, R86, R89, R90, R91, R92, R93, R94, R95, R103, R104, R105</t>
   </si>
 </sst>
 </file>
@@ -1044,10 +1043,6 @@
   </cellStyles>
   <dxfs count="11">
     <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1064,6 +1059,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1092,8 +1091,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:K48" totalsRowShown="0">
-  <autoFilter ref="A1:K48"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:K47" totalsRowShown="0">
+  <autoFilter ref="A1:K47"/>
   <sortState ref="A2:K56">
     <sortCondition ref="J2:J55" customList=".01uF,.1uF,.1uF,0R,0ZCJ0050AF2E,100K,100k,100nF,100nF,100nF,10K,120R,12K,12M,1751316,1K,1k,1uF,1uF,2.2K,20.1K,20.1k,200,200R,22,220R @ 100M,22pF,22uF,250,250k,39K,4.7K,4.7uF,47uF,698,7M-16.000MAAJ-T,93LC56C-I/SN"/>
   </sortState>
@@ -1102,13 +1101,13 @@
     <tableColumn id="2" name="Ref Des" dataDxfId="9"/>
     <tableColumn id="3" name="Qty" dataDxfId="8"/>
     <tableColumn id="4" name="Manufacturer" dataDxfId="7"/>
-    <tableColumn id="5" name="Mfg Part #" dataDxfId="0"/>
-    <tableColumn id="6" name="Description" dataDxfId="6"/>
-    <tableColumn id="7" name="Package" dataDxfId="5"/>
-    <tableColumn id="8" name="Type" dataDxfId="4"/>
-    <tableColumn id="9" name="Your Instructions" dataDxfId="3"/>
-    <tableColumn id="12" name="Value" dataDxfId="2"/>
-    <tableColumn id="13" name="Device" dataDxfId="1"/>
+    <tableColumn id="5" name="Mfg Part #" dataDxfId="6"/>
+    <tableColumn id="6" name="Description" dataDxfId="5"/>
+    <tableColumn id="7" name="Package" dataDxfId="4"/>
+    <tableColumn id="8" name="Type" dataDxfId="3"/>
+    <tableColumn id="9" name="Your Instructions" dataDxfId="2"/>
+    <tableColumn id="12" name="Value" dataDxfId="1"/>
+    <tableColumn id="13" name="Device" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1369,7 +1368,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1377,58 +1376,58 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L48"/>
+  <dimension ref="A1:L47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="89" zoomScaleNormal="89" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="L40" sqref="L40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.83203125" style="7"/>
-    <col min="2" max="2" width="37.6640625" style="7" customWidth="1"/>
-    <col min="3" max="3" width="8.83203125" style="7"/>
-    <col min="4" max="4" width="16.5" style="7" customWidth="1"/>
-    <col min="5" max="5" width="19.5" style="12" customWidth="1"/>
-    <col min="6" max="6" width="44.1640625" style="7" customWidth="1"/>
+    <col min="1" max="1" width="8.85546875" style="7"/>
+    <col min="2" max="2" width="37.7109375" style="7" customWidth="1"/>
+    <col min="3" max="3" width="8.85546875" style="7"/>
+    <col min="4" max="4" width="16.42578125" style="7" customWidth="1"/>
+    <col min="5" max="5" width="19.42578125" style="12" customWidth="1"/>
+    <col min="6" max="6" width="44.140625" style="7" customWidth="1"/>
     <col min="7" max="7" width="11" style="12" customWidth="1"/>
-    <col min="8" max="8" width="8.83203125" style="7"/>
-    <col min="9" max="9" width="18.1640625" style="7" customWidth="1"/>
-    <col min="10" max="10" width="25.5" style="6" customWidth="1"/>
-    <col min="11" max="11" width="19.83203125" style="6" customWidth="1"/>
-    <col min="12" max="12" width="40.1640625" style="6" customWidth="1"/>
-    <col min="13" max="15" width="8.83203125" style="6"/>
+    <col min="8" max="8" width="8.85546875" style="7"/>
+    <col min="9" max="9" width="18.140625" style="7" customWidth="1"/>
+    <col min="10" max="10" width="25.42578125" style="6" customWidth="1"/>
+    <col min="11" max="11" width="19.85546875" style="6" customWidth="1"/>
+    <col min="12" max="12" width="40.140625" style="6" customWidth="1"/>
+    <col min="13" max="15" width="8.85546875" style="6"/>
     <col min="16" max="16" width="11" style="6" bestFit="1" customWidth="1"/>
-    <col min="17" max="16384" width="8.83203125" style="6"/>
+    <col min="17" max="16384" width="8.85546875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="G1" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="H1" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="I1" s="5" t="s">
         <v>79</v>
-      </c>
-      <c r="H1" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>81</v>
       </c>
       <c r="J1" s="2" t="s">
         <v>1</v>
@@ -1437,7 +1436,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B2" s="8" t="s">
         <v>7</v>
       </c>
@@ -1445,77 +1444,77 @@
         <v>8</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>6</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B3" s="8" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C3" s="8">
         <v>4</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="G3" s="12" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>5</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B4" s="8" t="s">
-        <v>10</v>
+        <v>237</v>
       </c>
       <c r="C4" s="8">
         <v>11</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="G4" s="12" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="J4" s="1" t="s">
         <v>8</v>
@@ -1524,232 +1523,232 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B5" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C5" s="8">
         <v>1</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E5" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="G5" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="G5" s="12" t="s">
-        <v>90</v>
-      </c>
-      <c r="H5" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="K5" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11">
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B6" s="8" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C6" s="8">
         <v>2</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G6" s="12" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K6" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B7" s="8" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C7" s="8">
         <v>32</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="G7" s="12" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B8" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C8" s="8">
         <v>2</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="G8" s="12" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K8" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B9" s="8" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C9" s="8">
         <v>3</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="G9" s="12" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="H9" s="7" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K9" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B10" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C10" s="8">
         <v>1</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="G10" s="12" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="H10" s="7" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="K10" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11"/>
       <c r="B11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C11">
         <v>1</v>
       </c>
       <c r="D11" t="s">
+        <v>94</v>
+      </c>
+      <c r="E11" t="s">
+        <v>93</v>
+      </c>
+      <c r="F11" t="s">
+        <v>95</v>
+      </c>
+      <c r="G11" t="s">
         <v>96</v>
       </c>
-      <c r="E11" t="s">
-        <v>95</v>
-      </c>
-      <c r="F11" t="s">
-        <v>97</v>
-      </c>
-      <c r="G11" t="s">
-        <v>98</v>
-      </c>
       <c r="H11" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="I11"/>
       <c r="J11" t="s">
+        <v>27</v>
+      </c>
+      <c r="K11" t="s">
         <v>28</v>
       </c>
-      <c r="K11" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11">
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B12" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C12" s="8">
         <v>1</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E12" s="16">
         <v>1751316</v>
       </c>
       <c r="F12" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="G12" s="12" t="s">
         <v>100</v>
       </c>
-      <c r="G12" s="12" t="s">
-        <v>102</v>
-      </c>
       <c r="H12" s="7" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="J12" s="14">
         <v>1751316</v>
@@ -1758,143 +1757,143 @@
         <v>1751316</v>
       </c>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B13" s="8" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C13" s="8">
         <v>12</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E13" s="12" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="G13" s="12" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="H13" s="7" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K13" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B14" s="8" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C14" s="8">
         <v>18</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="G14" s="12" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="H14" s="7" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B15" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C15" s="8">
         <v>1</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="E15" s="12" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="G15" s="12" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="H15" s="7" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K15" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B16" s="8" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C16" s="8">
         <v>24</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="E16" s="12" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="G16" s="12" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="H16" s="7" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="K16" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:11">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B17" s="8" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C17" s="8">
         <v>3</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="E17" s="12" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="G17" s="12" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="H17" s="7" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="J17" s="1">
         <v>200</v>
@@ -1903,27 +1902,27 @@
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:11">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B18" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C18" s="8">
         <v>2</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E18" s="12" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="G18" s="12" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="H18" s="7" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="J18" s="1">
         <v>22</v>
@@ -1932,114 +1931,114 @@
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:11">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B19" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C19" s="8">
         <v>2</v>
       </c>
       <c r="D19" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E19" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="F19" t="s">
+        <v>83</v>
+      </c>
+      <c r="G19" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="F19" t="s">
-        <v>85</v>
-      </c>
-      <c r="G19" s="12" t="s">
-        <v>88</v>
-      </c>
       <c r="H19" s="7" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="J19" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="K19" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="K19" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11">
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B20" s="8" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C20" s="8">
         <v>4</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="E20" s="12" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="G20" s="12" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="H20" s="7" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="J20" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="K20" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="K20" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11">
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B21" s="8" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C21" s="8">
         <v>2</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="E21" s="12" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="G21" s="12" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="H21" s="7" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K21" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B22" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C22" s="8">
         <v>1</v>
       </c>
       <c r="D22" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="E22" s="12" t="s">
         <v>141</v>
       </c>
-      <c r="E22" s="12" t="s">
-        <v>143</v>
-      </c>
       <c r="F22" s="7" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="G22" s="12" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="H22" s="7" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="J22" s="1">
         <v>619</v>
@@ -2048,172 +2047,172 @@
         <v>9</v>
       </c>
     </row>
-    <row r="23" spans="1:11">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B23" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C23" s="8">
         <v>2</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E23" s="12" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="G23" s="12" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="H23" s="7" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K23" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:11">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B24" s="8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C24" s="8">
         <v>25</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="E24" s="12" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="G24" s="12" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="H24" s="7" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K24" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="1:11">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B25" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C25" s="8">
         <v>4</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E25" s="12" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="G25" s="12" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="H25" s="7" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K25" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="1:11">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B26" s="8" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C26" s="8">
         <v>7</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="E26" s="12" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="G26" s="12" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="H26" s="7" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="J26" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K26" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="K26" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11">
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B27" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C27" s="8">
         <v>1</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="E27" s="12" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="G27" s="12" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="H27" s="7" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="J27" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K27" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B28" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C28" s="8">
         <v>16</v>
       </c>
       <c r="D28" s="7" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="E28" s="12" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="G28" s="12" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="H28" s="7" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="J28" s="1">
         <v>698</v>
@@ -2222,147 +2221,162 @@
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="1:11">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29"/>
       <c r="B29" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C29">
         <v>1</v>
       </c>
       <c r="D29" t="s">
+        <v>94</v>
+      </c>
+      <c r="E29" t="s">
+        <v>21</v>
+      </c>
+      <c r="F29" t="s">
+        <v>236</v>
+      </c>
+      <c r="G29" t="s">
         <v>96</v>
       </c>
-      <c r="E29" t="s">
-        <v>22</v>
-      </c>
-      <c r="F29" t="s">
-        <v>239</v>
-      </c>
-      <c r="G29" t="s">
-        <v>98</v>
-      </c>
       <c r="H29" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="I29"/>
       <c r="J29" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K29" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B30" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C30" s="8">
         <v>1</v>
       </c>
       <c r="D30" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="E30" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="F30" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="G30" s="12" t="s">
         <v>149</v>
       </c>
-      <c r="E30" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="F30" s="7" t="s">
-        <v>150</v>
-      </c>
-      <c r="G30" s="12" t="s">
-        <v>151</v>
-      </c>
       <c r="H30" s="7" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="J30" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="K30" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B31" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C31" s="8">
         <v>1</v>
       </c>
       <c r="D31" s="7" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E31" s="12" t="s">
+        <v>170</v>
+      </c>
+      <c r="F31" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="I31" s="7" t="s">
         <v>172</v>
       </c>
-      <c r="F31" s="7" t="s">
-        <v>171</v>
-      </c>
-      <c r="I31" s="7" t="s">
-        <v>174</v>
-      </c>
       <c r="J31" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="K31" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B32" s="8" t="s">
-        <v>198</v>
+        <v>55</v>
       </c>
       <c r="C32" s="8">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="D32" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="E32" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="F32" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="G32" s="12" t="s">
+        <v>152</v>
+      </c>
+      <c r="H32" s="7" t="s">
+        <v>92</v>
       </c>
       <c r="J32" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="K32" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="K32" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="33" spans="2:12">
+    </row>
+    <row r="33" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B33" s="8" t="s">
         <v>57</v>
       </c>
       <c r="C33" s="8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D33" s="7" t="s">
-        <v>152</v>
-      </c>
-      <c r="E33" s="12" t="s">
-        <v>55</v>
+        <v>153</v>
+      </c>
+      <c r="E33" s="18" t="s">
+        <v>56</v>
       </c>
       <c r="F33" s="7" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="G33" s="12" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="H33" s="7" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="J33" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="K33" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="34" spans="2:12">
+    <row r="34" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B34" s="8" t="s">
         <v>59</v>
       </c>
       <c r="C34" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D34" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="E34" s="18" t="s">
-        <v>58</v>
+        <v>159</v>
+      </c>
+      <c r="E34" s="12" t="s">
+        <v>158</v>
       </c>
       <c r="F34" s="7" t="s">
         <v>156</v>
@@ -2371,7 +2385,7 @@
         <v>157</v>
       </c>
       <c r="H34" s="7" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="J34" s="1" t="s">
         <v>58</v>
@@ -2380,27 +2394,27 @@
         <v>58</v>
       </c>
     </row>
-    <row r="35" spans="2:12">
+    <row r="35" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B35" s="8" t="s">
         <v>61</v>
       </c>
       <c r="C35" s="8">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D35" s="7" t="s">
+        <v>159</v>
+      </c>
+      <c r="E35" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="F35" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="G35" s="12" t="s">
         <v>161</v>
       </c>
-      <c r="E35" s="12" t="s">
-        <v>160</v>
-      </c>
-      <c r="F35" s="7" t="s">
-        <v>158</v>
-      </c>
-      <c r="G35" s="12" t="s">
-        <v>159</v>
-      </c>
       <c r="H35" s="7" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="J35" s="1" t="s">
         <v>60</v>
@@ -2409,27 +2423,27 @@
         <v>60</v>
       </c>
     </row>
-    <row r="36" spans="2:12">
+    <row r="36" spans="2:12" ht="30" x14ac:dyDescent="0.25">
       <c r="B36" s="8" t="s">
         <v>63</v>
       </c>
       <c r="C36" s="8">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D36" s="7" t="s">
-        <v>161</v>
-      </c>
-      <c r="E36" s="18" t="s">
-        <v>62</v>
+        <v>159</v>
+      </c>
+      <c r="E36" s="12" t="s">
+        <v>162</v>
       </c>
       <c r="F36" s="7" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="G36" s="12" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="H36" s="7" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="J36" s="1" t="s">
         <v>62</v>
@@ -2438,7 +2452,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="37" spans="2:12" ht="28">
+    <row r="37" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B37" s="8" t="s">
         <v>65</v>
       </c>
@@ -2446,19 +2460,19 @@
         <v>1</v>
       </c>
       <c r="D37" s="7" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E37" s="12" t="s">
-        <v>164</v>
-      </c>
-      <c r="F37" s="7" t="s">
         <v>165</v>
       </c>
+      <c r="F37" s="13" t="s">
+        <v>166</v>
+      </c>
       <c r="G37" s="12" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="H37" s="7" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="J37" s="1" t="s">
         <v>64</v>
@@ -2467,65 +2481,65 @@
         <v>64</v>
       </c>
     </row>
-    <row r="38" spans="2:12">
+    <row r="38" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B38" s="8" t="s">
         <v>67</v>
       </c>
       <c r="C38" s="8">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="D38" s="7" t="s">
-        <v>161</v>
+        <v>121</v>
       </c>
       <c r="E38" s="12" t="s">
-        <v>167</v>
-      </c>
-      <c r="F38" s="13" t="s">
-        <v>168</v>
+        <v>120</v>
+      </c>
+      <c r="F38" s="15" t="s">
+        <v>122</v>
       </c>
       <c r="G38" s="12" t="s">
-        <v>169</v>
+        <v>87</v>
       </c>
       <c r="H38" s="7" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="J38" s="1" t="s">
         <v>66</v>
       </c>
       <c r="K38" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="39" spans="2:12">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="39" spans="2:12" ht="30" x14ac:dyDescent="0.25">
       <c r="B39" s="8" t="s">
         <v>69</v>
       </c>
       <c r="C39" s="8">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="D39" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="E39" s="12" t="s">
-        <v>122</v>
-      </c>
-      <c r="F39" s="15" t="s">
-        <v>124</v>
+        <v>117</v>
+      </c>
+      <c r="E39" s="12">
+        <v>1050170001</v>
+      </c>
+      <c r="F39" s="7" t="s">
+        <v>118</v>
       </c>
       <c r="G39" s="12" t="s">
-        <v>89</v>
+        <v>119</v>
       </c>
       <c r="H39" s="7" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="J39" s="1" t="s">
         <v>68</v>
       </c>
       <c r="K39" s="1" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="40" spans="2:12" ht="28">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="40" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B40" s="8" t="s">
         <v>71</v>
       </c>
@@ -2533,19 +2547,19 @@
         <v>1</v>
       </c>
       <c r="D40" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="E40" s="12">
-        <v>1050170001</v>
+        <v>173</v>
+      </c>
+      <c r="E40" s="12" t="s">
+        <v>70</v>
       </c>
       <c r="F40" s="7" t="s">
-        <v>120</v>
+        <v>174</v>
       </c>
       <c r="G40" s="12" t="s">
-        <v>121</v>
+        <v>175</v>
       </c>
       <c r="H40" s="7" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="J40" s="1" t="s">
         <v>70</v>
@@ -2553,234 +2567,205 @@
       <c r="K40" s="1" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="41" spans="2:12">
+      <c r="L40" s="6" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="41" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B41" s="8" t="s">
-        <v>73</v>
+        <v>168</v>
       </c>
       <c r="C41" s="8">
         <v>1</v>
       </c>
       <c r="D41" s="7" t="s">
-        <v>175</v>
+        <v>106</v>
       </c>
       <c r="E41" s="12" t="s">
-        <v>72</v>
+        <v>111</v>
       </c>
       <c r="F41" s="7" t="s">
-        <v>176</v>
+        <v>110</v>
       </c>
       <c r="G41" s="12" t="s">
-        <v>177</v>
+        <v>86</v>
       </c>
       <c r="H41" s="7" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="J41" s="1" t="s">
-        <v>72</v>
+        <v>108</v>
       </c>
       <c r="K41" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="L41" s="6" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="42" spans="2:12">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="42" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B42" s="8" t="s">
-        <v>170</v>
+        <v>102</v>
       </c>
       <c r="C42" s="8">
         <v>1</v>
       </c>
       <c r="D42" s="7" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E42" s="12" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="F42" s="7" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="G42" s="12" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="H42" s="7" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="J42" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="K42" s="1" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="43" spans="2:12">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="43" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B43" s="8" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C43" s="8">
         <v>1</v>
       </c>
       <c r="D43" s="7" t="s">
-        <v>108</v>
+        <v>115</v>
       </c>
       <c r="E43" s="12" t="s">
-        <v>107</v>
+        <v>114</v>
       </c>
       <c r="F43" s="7" t="s">
-        <v>109</v>
+        <v>116</v>
       </c>
       <c r="G43" s="12" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="H43" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="J43" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="K43" s="1" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="44" spans="2:12">
+        <v>92</v>
+      </c>
+      <c r="J43" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="K43" s="10" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="44" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B44" s="8" t="s">
-        <v>103</v>
+        <v>4</v>
       </c>
       <c r="C44" s="8">
         <v>1</v>
       </c>
       <c r="D44" s="7" t="s">
-        <v>117</v>
+        <v>144</v>
       </c>
       <c r="E44" s="12" t="s">
-        <v>116</v>
+        <v>142</v>
       </c>
       <c r="F44" s="7" t="s">
-        <v>118</v>
+        <v>143</v>
       </c>
       <c r="G44" s="12" t="s">
-        <v>88</v>
+        <v>145</v>
       </c>
       <c r="H44" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="J44" s="9" t="s">
-        <v>114</v>
-      </c>
-      <c r="K44" s="10" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="45" spans="2:12">
+        <v>92</v>
+      </c>
+      <c r="J44" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="K44" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="45" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B45" s="8" t="s">
-        <v>4</v>
+        <v>136</v>
       </c>
       <c r="C45" s="8">
         <v>1</v>
       </c>
       <c r="D45" s="7" t="s">
-        <v>146</v>
+        <v>115</v>
       </c>
       <c r="E45" s="12" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="F45" s="7" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="G45" s="12" t="s">
-        <v>147</v>
+        <v>87</v>
       </c>
       <c r="H45" s="7" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="J45" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="K45" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="46" spans="2:12">
+        <v>112</v>
+      </c>
+      <c r="K45" s="10" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="46" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B46" s="8" t="s">
-        <v>138</v>
+        <v>124</v>
       </c>
       <c r="C46" s="8">
         <v>1</v>
       </c>
       <c r="D46" s="7" t="s">
-        <v>117</v>
+        <v>126</v>
       </c>
       <c r="E46" s="12" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
       <c r="F46" s="7" t="s">
-        <v>140</v>
-      </c>
-      <c r="G46" s="12" t="s">
-        <v>89</v>
+        <v>125</v>
       </c>
       <c r="H46" s="7" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="J46" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="K46" s="10" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="47" spans="2:12">
+        <v>129</v>
+      </c>
+      <c r="K46" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="47" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B47" s="8" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="C47" s="8">
         <v>1</v>
       </c>
       <c r="D47" s="7" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="E47" s="12" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="F47" s="7" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="H47" s="7" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="J47" s="1" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="K47" s="1" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="48" spans="2:12">
-      <c r="B48" s="8" t="s">
-        <v>132</v>
-      </c>
-      <c r="C48" s="8">
-        <v>1</v>
-      </c>
-      <c r="D48" s="7" t="s">
-        <v>134</v>
-      </c>
-      <c r="E48" s="12" t="s">
-        <v>133</v>
-      </c>
-      <c r="F48" s="7" t="s">
         <v>135</v>
-      </c>
-      <c r="H48" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="J48" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="K48" s="1" t="s">
-        <v>137</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revert back to Submittable BOM
</commit_message>
<xml_diff>
--- a/CANnode/Output/BOM_Final.xlsx
+++ b/CANnode/Output/BOM_Final.xlsx
@@ -1,33 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="26221"/>
   <workbookPr autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\W2016\Desktop\RM42-CAN-Sensor-Node\CANnode\Output\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28785" windowHeight="17535"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28780" windowHeight="17540"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="240">
   <si>
     <t>Qty</t>
   </si>
@@ -59,6 +54,9 @@
     <t>RES0402</t>
   </si>
   <si>
+    <t>R86, R89, R90, R91, R92, R93, R94, R95, R103, R104, R105</t>
+  </si>
+  <si>
     <t>0ZCJ0050AF2E</t>
   </si>
   <si>
@@ -186,6 +184,9 @@
   </si>
   <si>
     <t>X1</t>
+  </si>
+  <si>
+    <t>DNP</t>
   </si>
   <si>
     <t>FDV302P</t>
@@ -620,6 +621,9 @@
     <t>R5,R6,R114</t>
   </si>
   <si>
+    <t>R59</t>
+  </si>
+  <si>
     <t>Vishay Dale</t>
   </si>
   <si>
@@ -741,9 +745,6 @@
   </si>
   <si>
     <t>Crystal 16MHZ</t>
-  </si>
-  <si>
-    <t>R59, R86, R89, R90, R91, R92, R93, R94, R95, R103, R104, R105</t>
   </si>
 </sst>
 </file>
@@ -1043,6 +1044,10 @@
   </cellStyles>
   <dxfs count="11">
     <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1059,10 +1064,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1091,8 +1092,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:K47" totalsRowShown="0">
-  <autoFilter ref="A1:K47"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:K48" totalsRowShown="0">
+  <autoFilter ref="A1:K48"/>
   <sortState ref="A2:K56">
     <sortCondition ref="J2:J55" customList=".01uF,.1uF,.1uF,0R,0ZCJ0050AF2E,100K,100k,100nF,100nF,100nF,10K,120R,12K,12M,1751316,1K,1k,1uF,1uF,2.2K,20.1K,20.1k,200,200R,22,220R @ 100M,22pF,22uF,250,250k,39K,4.7K,4.7uF,47uF,698,7M-16.000MAAJ-T,93LC56C-I/SN"/>
   </sortState>
@@ -1101,13 +1102,13 @@
     <tableColumn id="2" name="Ref Des" dataDxfId="9"/>
     <tableColumn id="3" name="Qty" dataDxfId="8"/>
     <tableColumn id="4" name="Manufacturer" dataDxfId="7"/>
-    <tableColumn id="5" name="Mfg Part #" dataDxfId="6"/>
-    <tableColumn id="6" name="Description" dataDxfId="5"/>
-    <tableColumn id="7" name="Package" dataDxfId="4"/>
-    <tableColumn id="8" name="Type" dataDxfId="3"/>
-    <tableColumn id="9" name="Your Instructions" dataDxfId="2"/>
-    <tableColumn id="12" name="Value" dataDxfId="1"/>
-    <tableColumn id="13" name="Device" dataDxfId="0"/>
+    <tableColumn id="5" name="Mfg Part #" dataDxfId="0"/>
+    <tableColumn id="6" name="Description" dataDxfId="6"/>
+    <tableColumn id="7" name="Package" dataDxfId="5"/>
+    <tableColumn id="8" name="Type" dataDxfId="4"/>
+    <tableColumn id="9" name="Your Instructions" dataDxfId="3"/>
+    <tableColumn id="12" name="Value" dataDxfId="2"/>
+    <tableColumn id="13" name="Device" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1368,7 +1369,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1376,58 +1377,58 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L47"/>
+  <dimension ref="A1:L48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="89" zoomScaleNormal="89" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="L40" sqref="L40"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" style="7"/>
-    <col min="2" max="2" width="37.7109375" style="7" customWidth="1"/>
-    <col min="3" max="3" width="8.85546875" style="7"/>
-    <col min="4" max="4" width="16.42578125" style="7" customWidth="1"/>
-    <col min="5" max="5" width="19.42578125" style="12" customWidth="1"/>
-    <col min="6" max="6" width="44.140625" style="7" customWidth="1"/>
+    <col min="1" max="1" width="8.83203125" style="7"/>
+    <col min="2" max="2" width="37.6640625" style="7" customWidth="1"/>
+    <col min="3" max="3" width="8.83203125" style="7"/>
+    <col min="4" max="4" width="16.5" style="7" customWidth="1"/>
+    <col min="5" max="5" width="19.5" style="12" customWidth="1"/>
+    <col min="6" max="6" width="44.1640625" style="7" customWidth="1"/>
     <col min="7" max="7" width="11" style="12" customWidth="1"/>
-    <col min="8" max="8" width="8.85546875" style="7"/>
-    <col min="9" max="9" width="18.140625" style="7" customWidth="1"/>
-    <col min="10" max="10" width="25.42578125" style="6" customWidth="1"/>
-    <col min="11" max="11" width="19.85546875" style="6" customWidth="1"/>
-    <col min="12" max="12" width="40.140625" style="6" customWidth="1"/>
-    <col min="13" max="15" width="8.85546875" style="6"/>
+    <col min="8" max="8" width="8.83203125" style="7"/>
+    <col min="9" max="9" width="18.1640625" style="7" customWidth="1"/>
+    <col min="10" max="10" width="25.5" style="6" customWidth="1"/>
+    <col min="11" max="11" width="19.83203125" style="6" customWidth="1"/>
+    <col min="12" max="12" width="40.1640625" style="6" customWidth="1"/>
+    <col min="13" max="15" width="8.83203125" style="6"/>
     <col min="16" max="16" width="11" style="6" bestFit="1" customWidth="1"/>
-    <col min="17" max="16384" width="8.85546875" style="6"/>
+    <col min="17" max="16384" width="8.83203125" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11">
       <c r="A1" s="3" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="G1" s="11" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="J1" s="2" t="s">
         <v>1</v>
@@ -1436,7 +1437,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11">
       <c r="B2" s="8" t="s">
         <v>7</v>
       </c>
@@ -1444,77 +1445,77 @@
         <v>8</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>6</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
       <c r="B3" s="8" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="C3" s="8">
         <v>4</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="G3" s="12" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>5</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
       <c r="B4" s="8" t="s">
-        <v>237</v>
+        <v>10</v>
       </c>
       <c r="C4" s="8">
         <v>11</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="G4" s="12" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="J4" s="1" t="s">
         <v>8</v>
@@ -1523,232 +1524,232 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11">
       <c r="B5" s="8" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C5" s="8">
         <v>1</v>
       </c>
       <c r="D5" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="G5" s="12" t="s">
         <v>90</v>
       </c>
-      <c r="E5" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="F5" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="G5" s="12" t="s">
-        <v>88</v>
-      </c>
       <c r="H5" s="7" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
       <c r="B6" s="8" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="C6" s="8">
         <v>2</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="G6" s="12" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="K6" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11">
       <c r="B7" s="8" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="C7" s="8">
         <v>32</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="G7" s="12" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
       <c r="B8" s="8" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C8" s="8">
         <v>2</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="G8" s="12" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="K8" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11">
       <c r="B9" s="8" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="C9" s="8">
         <v>3</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="G9" s="12" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="H9" s="7" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="K9" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11">
       <c r="B10" s="8" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C10" s="8">
         <v>1</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="G10" s="12" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="H10" s="7" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="K10" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11">
       <c r="A11"/>
       <c r="B11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C11">
         <v>1</v>
       </c>
       <c r="D11" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="E11" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="F11" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="G11" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="H11" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="I11"/>
       <c r="J11" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="K11" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
       <c r="B12" s="8" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C12" s="8">
         <v>1</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="E12" s="16">
         <v>1751316</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="G12" s="12" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="H12" s="7" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="J12" s="14">
         <v>1751316</v>
@@ -1757,143 +1758,143 @@
         <v>1751316</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11">
       <c r="B13" s="8" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="C13" s="8">
         <v>12</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="E13" s="12" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="G13" s="12" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="H13" s="7" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="K13" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11">
       <c r="B14" s="8" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="C14" s="8">
         <v>18</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="G14" s="12" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="H14" s="7" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11">
       <c r="B15" s="8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C15" s="8">
         <v>1</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="E15" s="12" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="G15" s="12" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="H15" s="7" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="K15" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11">
       <c r="B16" s="8" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="C16" s="8">
         <v>24</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="E16" s="12" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="F16" s="7" t="s">
+        <v>214</v>
+      </c>
+      <c r="G16" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="H16" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="J16" s="1" t="s">
         <v>211</v>
-      </c>
-      <c r="G16" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="H16" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="J16" s="1" t="s">
-        <v>208</v>
       </c>
       <c r="K16" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11">
       <c r="B17" s="8" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="C17" s="8">
         <v>3</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="E17" s="12" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="G17" s="12" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="H17" s="7" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="J17" s="1">
         <v>200</v>
@@ -1902,27 +1903,27 @@
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11">
       <c r="B18" s="8" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C18" s="8">
         <v>2</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="E18" s="12" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="G18" s="12" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="H18" s="7" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="J18" s="1">
         <v>22</v>
@@ -1931,114 +1932,114 @@
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11">
       <c r="B19" s="8" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C19" s="8">
         <v>2</v>
       </c>
       <c r="D19" t="s">
+        <v>87</v>
+      </c>
+      <c r="E19" s="17" t="s">
+        <v>86</v>
+      </c>
+      <c r="F19" t="s">
         <v>85</v>
       </c>
-      <c r="E19" s="17" t="s">
-        <v>84</v>
-      </c>
-      <c r="F19" t="s">
+      <c r="G19" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="H19" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="K19" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11">
+      <c r="B20" s="8" t="s">
         <v>83</v>
-      </c>
-      <c r="G19" s="12" t="s">
-        <v>86</v>
-      </c>
-      <c r="H19" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="J19" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="K19" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B20" s="8" t="s">
-        <v>81</v>
       </c>
       <c r="C20" s="8">
         <v>4</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="E20" s="12" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="G20" s="12" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="H20" s="7" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11">
       <c r="B21" s="8" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C21" s="8">
         <v>2</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="E21" s="12" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="G21" s="12" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="H21" s="7" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="K21" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11">
       <c r="B22" s="8" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C22" s="8">
         <v>1</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="E22" s="12" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="G22" s="12" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="H22" s="7" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="J22" s="1">
         <v>619</v>
@@ -2047,172 +2048,172 @@
         <v>9</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11">
       <c r="B23" s="8" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C23" s="8">
         <v>2</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="E23" s="12" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="G23" s="12" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="H23" s="7" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="K23" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11">
       <c r="B24" s="8" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C24" s="8">
         <v>25</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="E24" s="12" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="G24" s="12" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="H24" s="7" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="K24" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11">
       <c r="B25" s="8" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C25" s="8">
         <v>4</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="E25" s="12" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="G25" s="12" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="H25" s="7" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="K25" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11">
       <c r="B26" s="8" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C26" s="8">
         <v>7</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="E26" s="12" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="G26" s="12" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="H26" s="7" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11">
       <c r="B27" s="8" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C27" s="8">
         <v>1</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="E27" s="12" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="G27" s="12" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="H27" s="7" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="J27" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="K27" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11">
       <c r="B28" s="8" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C28" s="8">
         <v>16</v>
       </c>
       <c r="D28" s="7" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="E28" s="12" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
       <c r="G28" s="12" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="H28" s="7" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="J28" s="1">
         <v>698</v>
@@ -2221,162 +2222,147 @@
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11">
       <c r="A29"/>
       <c r="B29" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C29">
         <v>1</v>
       </c>
       <c r="D29" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="E29" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F29" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="G29" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="H29" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="I29"/>
       <c r="J29" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="K29" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11">
       <c r="B30" s="8" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C30" s="8">
         <v>1</v>
       </c>
       <c r="D30" s="7" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="E30" s="12" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F30" s="7" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="G30" s="12" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="H30" s="7" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="J30" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="K30" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11">
       <c r="B31" s="8" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C31" s="8">
         <v>1</v>
       </c>
       <c r="D31" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="E31" s="12" t="s">
+        <v>172</v>
+      </c>
+      <c r="F31" s="7" t="s">
         <v>171</v>
       </c>
-      <c r="E31" s="12" t="s">
-        <v>170</v>
-      </c>
-      <c r="F31" s="7" t="s">
-        <v>169</v>
-      </c>
       <c r="I31" s="7" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="J31" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="K31" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11">
       <c r="B32" s="8" t="s">
-        <v>55</v>
+        <v>198</v>
       </c>
       <c r="C32" s="8">
-        <v>2</v>
-      </c>
-      <c r="D32" s="7" t="s">
-        <v>150</v>
-      </c>
-      <c r="E32" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="F32" s="7" t="s">
-        <v>151</v>
-      </c>
-      <c r="G32" s="12" t="s">
-        <v>152</v>
-      </c>
-      <c r="H32" s="7" t="s">
-        <v>92</v>
+        <v>1</v>
       </c>
       <c r="J32" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="K32" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="33" spans="2:12" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="33" spans="2:12">
       <c r="B33" s="8" t="s">
         <v>57</v>
       </c>
       <c r="C33" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D33" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="E33" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="F33" s="7" t="s">
         <v>153</v>
       </c>
-      <c r="E33" s="18" t="s">
-        <v>56</v>
-      </c>
-      <c r="F33" s="7" t="s">
+      <c r="G33" s="12" t="s">
         <v>154</v>
       </c>
-      <c r="G33" s="12" t="s">
-        <v>155</v>
-      </c>
       <c r="H33" s="7" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="J33" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K33" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="34" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:12">
       <c r="B34" s="8" t="s">
         <v>59</v>
       </c>
       <c r="C34" s="8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D34" s="7" t="s">
-        <v>159</v>
-      </c>
-      <c r="E34" s="12" t="s">
-        <v>158</v>
+        <v>155</v>
+      </c>
+      <c r="E34" s="18" t="s">
+        <v>58</v>
       </c>
       <c r="F34" s="7" t="s">
         <v>156</v>
@@ -2385,7 +2371,7 @@
         <v>157</v>
       </c>
       <c r="H34" s="7" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="J34" s="1" t="s">
         <v>58</v>
@@ -2394,27 +2380,27 @@
         <v>58</v>
       </c>
     </row>
-    <row r="35" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:12">
       <c r="B35" s="8" t="s">
         <v>61</v>
       </c>
       <c r="C35" s="8">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D35" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="E35" s="12" t="s">
+        <v>160</v>
+      </c>
+      <c r="F35" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="G35" s="12" t="s">
         <v>159</v>
       </c>
-      <c r="E35" s="18" t="s">
-        <v>60</v>
-      </c>
-      <c r="F35" s="7" t="s">
-        <v>160</v>
-      </c>
-      <c r="G35" s="12" t="s">
-        <v>161</v>
-      </c>
       <c r="H35" s="7" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="J35" s="1" t="s">
         <v>60</v>
@@ -2423,27 +2409,27 @@
         <v>60</v>
       </c>
     </row>
-    <row r="36" spans="2:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:12">
       <c r="B36" s="8" t="s">
         <v>63</v>
       </c>
       <c r="C36" s="8">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D36" s="7" t="s">
-        <v>159</v>
-      </c>
-      <c r="E36" s="12" t="s">
+        <v>161</v>
+      </c>
+      <c r="E36" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="F36" s="7" t="s">
         <v>162</v>
       </c>
-      <c r="F36" s="7" t="s">
+      <c r="G36" s="12" t="s">
         <v>163</v>
       </c>
-      <c r="G36" s="12" t="s">
-        <v>164</v>
-      </c>
       <c r="H36" s="7" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="J36" s="1" t="s">
         <v>62</v>
@@ -2452,7 +2438,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="37" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:12" ht="28">
       <c r="B37" s="8" t="s">
         <v>65</v>
       </c>
@@ -2460,19 +2446,19 @@
         <v>1</v>
       </c>
       <c r="D37" s="7" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="E37" s="12" t="s">
+        <v>164</v>
+      </c>
+      <c r="F37" s="7" t="s">
         <v>165</v>
       </c>
-      <c r="F37" s="13" t="s">
+      <c r="G37" s="12" t="s">
         <v>166</v>
       </c>
-      <c r="G37" s="12" t="s">
-        <v>167</v>
-      </c>
       <c r="H37" s="7" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="J37" s="1" t="s">
         <v>64</v>
@@ -2481,65 +2467,65 @@
         <v>64</v>
       </c>
     </row>
-    <row r="38" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:12">
       <c r="B38" s="8" t="s">
         <v>67</v>
       </c>
       <c r="C38" s="8">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="D38" s="7" t="s">
-        <v>121</v>
+        <v>161</v>
       </c>
       <c r="E38" s="12" t="s">
-        <v>120</v>
-      </c>
-      <c r="F38" s="15" t="s">
-        <v>122</v>
+        <v>167</v>
+      </c>
+      <c r="F38" s="13" t="s">
+        <v>168</v>
       </c>
       <c r="G38" s="12" t="s">
-        <v>87</v>
+        <v>169</v>
       </c>
       <c r="H38" s="7" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="J38" s="1" t="s">
         <v>66</v>
       </c>
       <c r="K38" s="1" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="39" spans="2:12" ht="30" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="39" spans="2:12">
       <c r="B39" s="8" t="s">
         <v>69</v>
       </c>
       <c r="C39" s="8">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="D39" s="7" t="s">
-        <v>117</v>
-      </c>
-      <c r="E39" s="12">
-        <v>1050170001</v>
-      </c>
-      <c r="F39" s="7" t="s">
-        <v>118</v>
+        <v>123</v>
+      </c>
+      <c r="E39" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="F39" s="15" t="s">
+        <v>124</v>
       </c>
       <c r="G39" s="12" t="s">
-        <v>119</v>
+        <v>89</v>
       </c>
       <c r="H39" s="7" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="J39" s="1" t="s">
         <v>68</v>
       </c>
       <c r="K39" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="40" spans="2:12" x14ac:dyDescent="0.25">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="40" spans="2:12" ht="28">
       <c r="B40" s="8" t="s">
         <v>71</v>
       </c>
@@ -2547,19 +2533,19 @@
         <v>1</v>
       </c>
       <c r="D40" s="7" t="s">
-        <v>173</v>
-      </c>
-      <c r="E40" s="12" t="s">
-        <v>70</v>
+        <v>119</v>
+      </c>
+      <c r="E40" s="12">
+        <v>1050170001</v>
       </c>
       <c r="F40" s="7" t="s">
-        <v>174</v>
+        <v>120</v>
       </c>
       <c r="G40" s="12" t="s">
-        <v>175</v>
+        <v>121</v>
       </c>
       <c r="H40" s="7" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="J40" s="1" t="s">
         <v>70</v>
@@ -2567,205 +2553,234 @@
       <c r="K40" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="L40" s="6" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="41" spans="2:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="41" spans="2:12">
       <c r="B41" s="8" t="s">
-        <v>168</v>
+        <v>73</v>
       </c>
       <c r="C41" s="8">
         <v>1</v>
       </c>
       <c r="D41" s="7" t="s">
-        <v>106</v>
+        <v>175</v>
       </c>
       <c r="E41" s="12" t="s">
-        <v>111</v>
+        <v>72</v>
       </c>
       <c r="F41" s="7" t="s">
-        <v>110</v>
+        <v>176</v>
       </c>
       <c r="G41" s="12" t="s">
-        <v>86</v>
+        <v>177</v>
       </c>
       <c r="H41" s="7" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="J41" s="1" t="s">
-        <v>108</v>
+        <v>72</v>
       </c>
       <c r="K41" s="1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="42" spans="2:12" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+      <c r="L41" s="6" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="42" spans="2:12">
       <c r="B42" s="8" t="s">
-        <v>102</v>
+        <v>170</v>
       </c>
       <c r="C42" s="8">
         <v>1</v>
       </c>
       <c r="D42" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="E42" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="F42" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="G42" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="H42" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="J42" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="K42" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="E42" s="12" t="s">
-        <v>105</v>
-      </c>
-      <c r="F42" s="7" t="s">
-        <v>107</v>
-      </c>
-      <c r="G42" s="12" t="s">
-        <v>86</v>
-      </c>
-      <c r="H42" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="J42" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="K42" s="1" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="43" spans="2:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="43" spans="2:12">
       <c r="B43" s="8" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="C43" s="8">
         <v>1</v>
       </c>
       <c r="D43" s="7" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="E43" s="12" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="F43" s="7" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="G43" s="12" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="H43" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="J43" s="9" t="s">
-        <v>112</v>
-      </c>
-      <c r="K43" s="10" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="44" spans="2:12" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+      <c r="J43" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="K43" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="44" spans="2:12">
       <c r="B44" s="8" t="s">
-        <v>4</v>
+        <v>103</v>
       </c>
       <c r="C44" s="8">
         <v>1</v>
       </c>
       <c r="D44" s="7" t="s">
-        <v>144</v>
+        <v>117</v>
       </c>
       <c r="E44" s="12" t="s">
-        <v>142</v>
+        <v>116</v>
       </c>
       <c r="F44" s="7" t="s">
-        <v>143</v>
+        <v>118</v>
       </c>
       <c r="G44" s="12" t="s">
-        <v>145</v>
+        <v>88</v>
       </c>
       <c r="H44" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="J44" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="K44" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="45" spans="2:12" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+      <c r="J44" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="K44" s="10" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="45" spans="2:12">
       <c r="B45" s="8" t="s">
-        <v>136</v>
+        <v>4</v>
       </c>
       <c r="C45" s="8">
         <v>1</v>
       </c>
       <c r="D45" s="7" t="s">
-        <v>115</v>
+        <v>146</v>
       </c>
       <c r="E45" s="12" t="s">
-        <v>137</v>
+        <v>144</v>
       </c>
       <c r="F45" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="G45" s="12" t="s">
+        <v>147</v>
+      </c>
+      <c r="H45" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="J45" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="K45" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="46" spans="2:12">
+      <c r="B46" s="8" t="s">
         <v>138</v>
-      </c>
-      <c r="G45" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="H45" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="J45" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="K45" s="10" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="46" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B46" s="8" t="s">
-        <v>124</v>
       </c>
       <c r="C46" s="8">
         <v>1</v>
       </c>
       <c r="D46" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="E46" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="F46" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="G46" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="H46" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="J46" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="K46" s="10" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="47" spans="2:12">
+      <c r="B47" s="8" t="s">
         <v>126</v>
-      </c>
-      <c r="E46" s="12" t="s">
-        <v>127</v>
-      </c>
-      <c r="F46" s="7" t="s">
-        <v>125</v>
-      </c>
-      <c r="H46" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="J46" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="K46" s="1" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="47" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B47" s="8" t="s">
-        <v>130</v>
       </c>
       <c r="C47" s="8">
         <v>1</v>
       </c>
       <c r="D47" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="E47" s="12" t="s">
+        <v>129</v>
+      </c>
+      <c r="F47" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="H47" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="J47" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="K47" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="48" spans="2:12">
+      <c r="B48" s="8" t="s">
         <v>132</v>
       </c>
-      <c r="E47" s="12" t="s">
-        <v>131</v>
-      </c>
-      <c r="F47" s="7" t="s">
+      <c r="C48" s="8">
+        <v>1</v>
+      </c>
+      <c r="D48" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="E48" s="12" t="s">
         <v>133</v>
       </c>
-      <c r="H47" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="J47" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="K47" s="1" t="s">
+      <c r="F48" s="7" t="s">
         <v>135</v>
+      </c>
+      <c r="H48" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="J48" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="K48" s="1" t="s">
+        <v>137</v>
       </c>
     </row>
   </sheetData>

</xml_diff>